<commit_message>
Slight changes to validation
</commit_message>
<xml_diff>
--- a/atomica/framework_template.xlsx
+++ b/atomica/framework_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\atomica\core\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\atomica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B003D609-37F1-48F5-AB7E-2A3C78C86A81}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C795E81-E1CC-4408-A8B4-450E871C1F2B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -683,6 +683,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -718,13 +732,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -733,13 +740,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1096,8 +1096,8 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,7 +1199,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,7 +1251,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,7 +1295,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D1048576">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>AND(#REF!&lt;&gt;"",NOT(D2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5410,7 +5410,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048576">
-    <cfRule type="expression" dxfId="3" priority="8">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>AND(#REF!&lt;&gt;"",NOT(F2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5461,8 +5461,8 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5523,7 +5523,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J1048576">
-    <cfRule type="expression" dxfId="0" priority="9">
+    <cfRule type="expression" dxfId="1" priority="9">
       <formula>AND(#REF!&lt;&gt;"",NOT(J2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add links to default
</commit_message>
<xml_diff>
--- a/atomica/framework_template.xlsx
+++ b/atomica/framework_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\atomica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/atomica/atomica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B70881C-8EE5-453E-B4E4-098146697AB7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{54DEED03-B4C4-E44F-BDB8-5B0CDAB02763}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -28,54 +28,41 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Romesh</author>
+    <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{32DD1623-256E-410E-A864-AB07B61C4590}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{6D054FAC-31EB-B64A-AAB6-7FC00BC1104B}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Romesh:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
+          <t>For instructions on how to fill this out, please see cascade.tools/ug-frw-databookpages</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{E514681C-6E27-134C-B5D5-E0E6533607E9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">
-Use the code name to assign Compartments, Characteristics, and Parameters to a particular sheet in the databook</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{02FCBC89-37EE-4BD9-AFD7-1CA498C0A432}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
+          <t xml:space="preserve">For instructions on how to fill this out, please see </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Romesh:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This is the name of the sheet that will appear in the 'Sheets' tab of the databook</t>
+          <t>cascade.tools/ug-frw-databookpages</t>
         </r>
       </text>
     </comment>
@@ -89,42 +76,167 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{8F11EEB6-017C-4E97-8DFB-6E8BA3F55C2C}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{96AF6E9C-859C-7B41-8729-FDE8C2B2F20E}">
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This is a short 'code name' for the compartment - it should be lower case with no spaces e.g. 'sus'</t>
+          <t xml:space="preserve">The code name should be in lower case without spaces.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">For </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">further instructions on how to fill this out, please see cascade.tools/ug-frw-compartments
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{18044106-CF0A-4F46-AE9F-654B913C6CA3}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{8A61F6F3-E058-3D4F-8B1B-678D114AC818}">
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The 'Display name' will label the compartment on plots, so it should be descriptive e.g. 'Susceptible'</t>
+          <t xml:space="preserve">The display name appears on plots and other outputs.  It should be in sentence case. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>For further instructions on how to fill this out, please see cascade.tools/ug-frw-compartments</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{69690E77-E19A-4C62-A1A8-7A79BC1C6D8C}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{8F3D6D32-534D-6144-9E9E-E21FE71DE45B}">
       <text>
         <r>
           <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>For further instructions on how to fill this out, please see cascade.tools/ug-frw-compartments</t>
+        </r>
+        <r>
+          <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>If you want this compartment to appear in the databook for data entry, then specify one of the datasheet code names (from the 'Databook Pages' sheet) here</t>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">This column optionally marks whether a data-input section should
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">appear for this compartment in a custom databook sheet, if allowed
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">to appear at all according to 'databook order'.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Each value should be a code name for a desired page defined in
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">the 'custom databook pages' worksheet page.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">If a cell is left empty, the enabled data-input section should appear
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>in a default databook page dedicated to state variables.</t>
         </r>
       </text>
     </comment>
@@ -138,27 +250,36 @@
     <author>Romesh</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{18A5064E-3D3F-4E47-AB28-08E3744C6678}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00132119-CF85-A042-A3DF-E85CCB0207F5}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Romesh:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">The transition matrix specifies which parameters govern transitions between compartments. Entries in this matrix should correspond to parameter Code Names (cells will be red if the parameter name cannot be found on the Parameters sheet).
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-The transition matrix specifies which transitions exist and which parameter governs them. Transitions go from row to column</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">For further instructions on how to fill this out, please see cascade.tools/ug-frw-transitions
+</t>
         </r>
       </text>
     </comment>
@@ -172,68 +293,368 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{A81A74DD-AC0E-4B65-846B-CB2954186FEC}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{4F6398C2-8318-CD48-BCB8-6976B8150986}">
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This is a short 'code name' for the characteristic - it should be lower case with no spaces e.g. 'all_dx'</t>
+          <t xml:space="preserve">The code name should be in lower case without spaces.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">For further instructions on how to fill this out, please see cascade.tools/ug-frw-characteristics
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{57EA8209-4B86-41FB-BF49-4A6D4754AB5F}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{61BE71C1-9BAB-FE4A-B84D-D21869DA7F1B}">
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">The 'Display name' will label the characteristic on plots, so it should be descriptive e.g. 'Aware of diagnosis' </t>
+          <t xml:space="preserve">The display name will appear in plots and other outputs. It should be in sentence case.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>For further instructions on how to fill this out, please see cascade.tools/ug-frw-characteristics</t>
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{6201EA2B-5CE9-45D3-ABC5-5BC441C9B026}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{E1CBF276-EF66-FE4F-ACBC-37EC265A8DC4}">
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Specify a comma separated list of compartment and characteristics to include e.g. 'dx,tx'</t>
+          <t xml:space="preserve">This column is for the 'components' of a cascade characteristic.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">A component is either a compartment or a characteristic that has
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">been previously defined, i.e. in a previous row, and should be
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">listed in this (and appropriate subsequent columns) by 'Code Name'.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">For example, characteristic 'infected' may include 'dis_stage_1',
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">'dis_stage_2' and 'dis_advanced', where 'dis_advanced' is another
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">previously-defined characteristic including 'dis_stage_3' and
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">'dis_stage_4'.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">In an example model, 'infected' would track population size summed
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">across the four 'dis_stage' states.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Note: If two or more components are listed in the same column, they
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">must be separated by a comma.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>For further instructions on how to fill this out, please see cascade.tools/ug-frw-characteristics</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{7BD7B4BC-A36F-458A-A3A5-AFA478F72DEB}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{6C6FE8A6-8963-534F-A006-8569FB636B02}">
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>If you want this characteristic to correspond to a fraction (e.g. prevalance) then specify the denominator here. For example, a characteristic for prevalance might have components that include all infected people, and a denominator which consists of all people. The denominator should be a single compartment or characteristic, not a list</t>
+          <t xml:space="preserve">This column defines a 'denominator' attribute for a 'charac' item.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>For further instructions on how to fill this out, please see cascade.tools/ug-frw-characteristics</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{559607C2-31DF-4F19-8B38-ADD8E67B050A}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{71C55B05-E609-5E49-9D2C-CEF4F70CB97A}">
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>If you want this characteristic to appear in the databook for data entry, then specify one of the datasheet code names (from the 'Databook Pages' sheet) here</t>
+          <t xml:space="preserve">This column optionally marks whether a data-input section should
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">appear for this characteristic in a custom databook sheet, if allowed
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">to appear at all according to 'databook order'.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Each value should be a code name for a desired page defined in
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">the 'custom databook pages' worksheet page.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">If a cell is left empty, the enabled data-input section should appear
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">in a default databook page dedicated to state variables.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">For further instructions on how to fill this out, please see cascade.tools/ug-frw-characteristics
+</t>
         </r>
       </text>
     </comment>
@@ -247,120 +668,363 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{140756B8-9EBA-40C4-98A1-F91289280755}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00B994F2-88D7-014A-BA4B-CC10C0C357E5}">
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This is a short 'code name' for the parameter - it should be lower case with no spaces e.g. 'dx_rate'</t>
+          <t xml:space="preserve">The code name should be in lower case without spaces.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">For further instructions on how to fill this out, please see cascade.tools/ug-frw-parameters
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{88893BC8-8DD6-4669-A22B-E608B0618831}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{191B4A06-2F60-9441-A611-5E79792EC378}">
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">The 'Display name' will label the parameter on plots, so it should be descriptive e.g. 'Diagnosis rate'' </t>
+          <t xml:space="preserve">The display name will appear in plots and other outputs. It should be in sentence case.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>For further instructions on how to fill this out, please see cascade.tools/ug-frw-paramters</t>
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{EF5E3AFE-CA03-46C5-8AFC-2AC6046E3E09}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{324F41BE-5F5B-6449-85BF-E9B6DE881E69}">
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Specify the units for the parameter. Generally, it would be 'probability' for the probability of an individual making a transition over a 1 year period, or 'number' for the number of people that transition over a 1 year period</t>
+          <t xml:space="preserve">This column defines a 'format' attribute for a 'par' item.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>For further instructions on how to fill this out, please see cascade.tools/ug-frw-parameters</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{FCE4BAB8-A6E9-4C37-855F-51EEAFF610F3}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{70D87E64-159E-C444-9382-0A02DDCDDA05}">
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>If you specify a default value, it will automatically appear in the databook (but it can be subsequently changed)</t>
+          <t xml:space="preserve">This column defines a 'default_value' attribute for a 'par' item.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>For further instructions on how to fill this out, please see cascade.tools/ug-frw-parameters</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{F7DF6DA5-307D-42BB-80B5-CEE9AB8ED752}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{7779E86D-FEF5-2E4A-BD10-6FCBEBED6FF0}">
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>If you specify a minimum value, the parameter will never drop below this value. If included, it would typically be 0</t>
+          <t xml:space="preserve">This column defines a 'min' attribute for a 'par' item.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>For further instructions on how to fill this out, please see cascade.tools/ug-frw-parameters</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{4C3AB2C0-9D0C-4C0E-9CF0-D571224FE5BD}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{CB217CB7-86BB-2047-8483-468731597977}">
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>If you specify a maximum value, the parameter will never exceed this value. A common use would be to ensure that a probability cannot be larger than 1</t>
+          <t xml:space="preserve">This column defines a 'max' attribute for a 'par' item.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>For further instructions on how to fill this out, please see cascade.tools/ug-frw-parameters</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{98B9E77F-8634-4220-9AE2-2EB54A125949}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{3D75FA66-FF9A-EE4B-8444-1DA24C9818B1}">
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>If a parameter is computed dynamically as a function, enter the function here</t>
+          <t xml:space="preserve">This column defines a 'func' attribute for a 'par' item.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>For further instructions on how to fill this out, please see cascade.tools/ug-frw-parameters</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{974FC231-C2BA-4000-88CD-AB6CE23C45D0}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{9565A77B-E7BD-5940-B155-E5CEB8E6ACE0}">
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>If a parameter is marked as an impact, then it is considered eligible for programs will appear in the program book</t>
+          <t xml:space="preserve">If set to 'y', the parameter can be targeted by programs, and it will appear in the program book for any projects using this framework
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>For further instructions on how to fill this out, please see cascade.tools/ug-frw-parameters</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{9AB3D83C-D0BC-4583-B5B1-006FE7C2562F}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{F083A827-2D72-404B-905A-72224B220C6E}">
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>If you want this parameter to appear in the databook for data entry, then specify one of the datasheet code names (from the 'Databook Pages' sheet) here</t>
+          <t xml:space="preserve">This column optionally marks whether a data-input section should appear for this parameter in a custom databook sheet, if allowed to appear at all according to 'databook order'.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Each value should be a code name for a desired page defined in the 'custom databook pages' worksheet page. If a cell is left empty, the enabled data-input section should appear in a default databook page dedicated to parameters.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">For further instructions on how to fill this out, please see cascade.tools/ug-frw-parameters 
+</t>
         </r>
       </text>
     </comment>
@@ -378,23 +1042,42 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Romesh:</t>
+          <t xml:space="preserve">Specify the name of your cascade in this cell. In the cells below, specify the names of your cascade's stages
+</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Specify the name of your cascade in this cell. In the cells below, specify the names of your cascade's stages</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>For further instructions on how to fill this out, please see cascade.tools/ug-frw-cascades</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
@@ -402,23 +1085,42 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Romesh:</t>
+          <t xml:space="preserve">In this column, specify which compartments and characteristics make up each cascade stage. You should specify them as a comma separated list of code names e.g., 'sus, inf, rec'
+</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-In this column, specify which compartments and characteristics make up each cascade stage. You should specify them as a comma separated list of code names e.g., 'sus, inf, rec'</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>For further instructions on how to fill this out, please see cascade.tools/ug-frw-cascades</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
@@ -427,7 +1129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Code Name</t>
   </si>
@@ -466,9 +1168,6 @@
   </si>
   <si>
     <t>Template</t>
-  </si>
-  <si>
-    <t>This is a template cascade</t>
   </si>
   <si>
     <t>stocks</t>
@@ -540,26 +1239,26 @@
     <t>Use this file to specify the structure of your model. Any extra sheets will be ignored, so you can include other information in them</t>
   </si>
   <si>
-    <t>Default value</t>
+    <t>Targetable</t>
   </si>
   <si>
-    <t>Minimum value</t>
+    <t>This is a template cascade. For instructions on how to fill it out, please see: cascade.tools/user-guide</t>
   </si>
   <si>
-    <t>Maximum value</t>
+    <t>Default Value</t>
   </si>
   <si>
-    <t>Databook page</t>
+    <t>Minimum Value</t>
   </si>
   <si>
-    <t>Targetable</t>
+    <t>Maximum Value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -576,23 +1275,50 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color indexed="81"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -634,7 +1360,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1052,16 +1785,16 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="97.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="97.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -1069,75 +1802,75 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="234.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="234.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
         <v>26</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1154,42 +1887,42 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1206,23 +1939,23 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1230,7 +1963,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1238,12 +1971,12 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C1048576">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="9" priority="7">
       <formula>AND(#REF!&lt;&gt;"",NOT(C2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1289,16 +2022,14 @@
   </sheetPr>
   <dimension ref="A1:OH398"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:398" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:398" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -2891,2383 +3622,2383 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:398" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="str">
         <f>IF(Compartments!$A2&lt;&gt;"",Compartments!$A2,"")</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:398" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="str">
         <f>IF(Compartments!$A3&lt;&gt;"",Compartments!$A3,"")</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:398" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="str">
         <f>IF(Compartments!$A4&lt;&gt;"",Compartments!$A4,"")</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:398" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="str">
         <f>IF(Compartments!$A5&lt;&gt;"",Compartments!$A5,"")</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:398" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="str">
         <f>IF(Compartments!$A6&lt;&gt;"",Compartments!$A6,"")</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:398" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="str">
         <f>IF(Compartments!$A7&lt;&gt;"",Compartments!$A7,"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:398" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="str">
         <f>IF(Compartments!$A8&lt;&gt;"",Compartments!$A8,"")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:398" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="str">
         <f>IF(Compartments!$A9&lt;&gt;"",Compartments!$A9,"")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:398" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="str">
         <f>IF(Compartments!$A10&lt;&gt;"",Compartments!$A10,"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:398" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="str">
         <f>IF(Compartments!$A11&lt;&gt;"",Compartments!$A11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:398" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="str">
         <f>IF(Compartments!$A12&lt;&gt;"",Compartments!$A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:398" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="str">
         <f>IF(Compartments!$A13&lt;&gt;"",Compartments!$A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:398" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="str">
         <f>IF(Compartments!$A14&lt;&gt;"",Compartments!$A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:398" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="str">
         <f>IF(Compartments!$A15&lt;&gt;"",Compartments!$A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:398" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="str">
         <f>IF(Compartments!$A16&lt;&gt;"",Compartments!$A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="str">
         <f>IF(Compartments!$A17&lt;&gt;"",Compartments!$A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="str">
         <f>IF(Compartments!$A18&lt;&gt;"",Compartments!$A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="str">
         <f>IF(Compartments!$A19&lt;&gt;"",Compartments!$A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="str">
         <f>IF(Compartments!$A20&lt;&gt;"",Compartments!$A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="str">
         <f>IF(Compartments!$A21&lt;&gt;"",Compartments!$A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="str">
         <f>IF(Compartments!$A22&lt;&gt;"",Compartments!$A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="str">
         <f>IF(Compartments!$A23&lt;&gt;"",Compartments!$A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="str">
         <f>IF(Compartments!$A24&lt;&gt;"",Compartments!$A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="str">
         <f>IF(Compartments!$A25&lt;&gt;"",Compartments!$A25,"")</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="str">
         <f>IF(Compartments!$A26&lt;&gt;"",Compartments!$A26,"")</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="str">
         <f>IF(Compartments!$A27&lt;&gt;"",Compartments!$A27,"")</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="str">
         <f>IF(Compartments!$A28&lt;&gt;"",Compartments!$A28,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="str">
         <f>IF(Compartments!$A29&lt;&gt;"",Compartments!$A29,"")</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="str">
         <f>IF(Compartments!$A30&lt;&gt;"",Compartments!$A30,"")</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="str">
         <f>IF(Compartments!$A31&lt;&gt;"",Compartments!$A31,"")</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="str">
         <f>IF(Compartments!$A32&lt;&gt;"",Compartments!$A32,"")</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="str">
         <f>IF(Compartments!$A33&lt;&gt;"",Compartments!$A33,"")</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="str">
         <f>IF(Compartments!$A34&lt;&gt;"",Compartments!$A34,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="str">
         <f>IF(Compartments!$A35&lt;&gt;"",Compartments!$A35,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="str">
         <f>IF(Compartments!$A36&lt;&gt;"",Compartments!$A36,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="str">
         <f>IF(Compartments!$A37&lt;&gt;"",Compartments!$A37,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="str">
         <f>IF(Compartments!$A38&lt;&gt;"",Compartments!$A38,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="str">
         <f>IF(Compartments!$A39&lt;&gt;"",Compartments!$A39,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="str">
         <f>IF(Compartments!$A40&lt;&gt;"",Compartments!$A40,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="str">
         <f>IF(Compartments!$A41&lt;&gt;"",Compartments!$A41,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="str">
         <f>IF(Compartments!$A42&lt;&gt;"",Compartments!$A42,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="str">
         <f>IF(Compartments!$A43&lt;&gt;"",Compartments!$A43,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="str">
         <f>IF(Compartments!$A44&lt;&gt;"",Compartments!$A44,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="str">
         <f>IF(Compartments!$A45&lt;&gt;"",Compartments!$A45,"")</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="str">
         <f>IF(Compartments!$A46&lt;&gt;"",Compartments!$A46,"")</f>
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="str">
         <f>IF(Compartments!$A47&lt;&gt;"",Compartments!$A47,"")</f>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="str">
         <f>IF(Compartments!$A48&lt;&gt;"",Compartments!$A48,"")</f>
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="str">
         <f>IF(Compartments!$A49&lt;&gt;"",Compartments!$A49,"")</f>
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="str">
         <f>IF(Compartments!$A50&lt;&gt;"",Compartments!$A50,"")</f>
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="str">
         <f>IF(Compartments!$A51&lt;&gt;"",Compartments!$A51,"")</f>
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="str">
         <f>IF(Compartments!$A52&lt;&gt;"",Compartments!$A52,"")</f>
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="str">
         <f>IF(Compartments!$A53&lt;&gt;"",Compartments!$A53,"")</f>
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="str">
         <f>IF(Compartments!$A54&lt;&gt;"",Compartments!$A54,"")</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="str">
         <f>IF(Compartments!$A55&lt;&gt;"",Compartments!$A55,"")</f>
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="str">
         <f>IF(Compartments!$A56&lt;&gt;"",Compartments!$A56,"")</f>
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="str">
         <f>IF(Compartments!$A57&lt;&gt;"",Compartments!$A57,"")</f>
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="str">
         <f>IF(Compartments!$A58&lt;&gt;"",Compartments!$A58,"")</f>
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="str">
         <f>IF(Compartments!$A59&lt;&gt;"",Compartments!$A59,"")</f>
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="str">
         <f>IF(Compartments!$A60&lt;&gt;"",Compartments!$A60,"")</f>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="str">
         <f>IF(Compartments!$A61&lt;&gt;"",Compartments!$A61,"")</f>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="str">
         <f>IF(Compartments!$A62&lt;&gt;"",Compartments!$A62,"")</f>
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="str">
         <f>IF(Compartments!$A63&lt;&gt;"",Compartments!$A63,"")</f>
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="str">
         <f>IF(Compartments!$A64&lt;&gt;"",Compartments!$A64,"")</f>
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="str">
         <f>IF(Compartments!$A65&lt;&gt;"",Compartments!$A65,"")</f>
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="str">
         <f>IF(Compartments!$A66&lt;&gt;"",Compartments!$A66,"")</f>
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="str">
         <f>IF(Compartments!$A67&lt;&gt;"",Compartments!$A67,"")</f>
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="str">
         <f>IF(Compartments!$A68&lt;&gt;"",Compartments!$A68,"")</f>
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="str">
         <f>IF(Compartments!$A69&lt;&gt;"",Compartments!$A69,"")</f>
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="str">
         <f>IF(Compartments!$A70&lt;&gt;"",Compartments!$A70,"")</f>
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="str">
         <f>IF(Compartments!$A71&lt;&gt;"",Compartments!$A71,"")</f>
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="str">
         <f>IF(Compartments!$A72&lt;&gt;"",Compartments!$A72,"")</f>
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="str">
         <f>IF(Compartments!$A73&lt;&gt;"",Compartments!$A73,"")</f>
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="str">
         <f>IF(Compartments!$A74&lt;&gt;"",Compartments!$A74,"")</f>
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="str">
         <f>IF(Compartments!$A75&lt;&gt;"",Compartments!$A75,"")</f>
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="str">
         <f>IF(Compartments!$A76&lt;&gt;"",Compartments!$A76,"")</f>
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="str">
         <f>IF(Compartments!$A77&lt;&gt;"",Compartments!$A77,"")</f>
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="str">
         <f>IF(Compartments!$A78&lt;&gt;"",Compartments!$A78,"")</f>
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="str">
         <f>IF(Compartments!$A79&lt;&gt;"",Compartments!$A79,"")</f>
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="str">
         <f>IF(Compartments!$A80&lt;&gt;"",Compartments!$A80,"")</f>
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="str">
         <f>IF(Compartments!$A81&lt;&gt;"",Compartments!$A81,"")</f>
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="str">
         <f>IF(Compartments!$A82&lt;&gt;"",Compartments!$A82,"")</f>
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="str">
         <f>IF(Compartments!$A83&lt;&gt;"",Compartments!$A83,"")</f>
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="str">
         <f>IF(Compartments!$A84&lt;&gt;"",Compartments!$A84,"")</f>
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="str">
         <f>IF(Compartments!$A85&lt;&gt;"",Compartments!$A85,"")</f>
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="str">
         <f>IF(Compartments!$A86&lt;&gt;"",Compartments!$A86,"")</f>
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="str">
         <f>IF(Compartments!$A87&lt;&gt;"",Compartments!$A87,"")</f>
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="str">
         <f>IF(Compartments!$A88&lt;&gt;"",Compartments!$A88,"")</f>
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="str">
         <f>IF(Compartments!$A89&lt;&gt;"",Compartments!$A89,"")</f>
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="str">
         <f>IF(Compartments!$A90&lt;&gt;"",Compartments!$A90,"")</f>
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="str">
         <f>IF(Compartments!$A91&lt;&gt;"",Compartments!$A91,"")</f>
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="str">
         <f>IF(Compartments!$A92&lt;&gt;"",Compartments!$A92,"")</f>
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="str">
         <f>IF(Compartments!$A93&lt;&gt;"",Compartments!$A93,"")</f>
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="str">
         <f>IF(Compartments!$A94&lt;&gt;"",Compartments!$A94,"")</f>
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="str">
         <f>IF(Compartments!$A95&lt;&gt;"",Compartments!$A95,"")</f>
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="str">
         <f>IF(Compartments!$A96&lt;&gt;"",Compartments!$A96,"")</f>
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="str">
         <f>IF(Compartments!$A97&lt;&gt;"",Compartments!$A97,"")</f>
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="str">
         <f>IF(Compartments!$A98&lt;&gt;"",Compartments!$A98,"")</f>
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="str">
         <f>IF(Compartments!$A99&lt;&gt;"",Compartments!$A99,"")</f>
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="str">
         <f>IF(Compartments!$A100&lt;&gt;"",Compartments!$A100,"")</f>
         <v/>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="str">
         <f>IF(Compartments!$A101&lt;&gt;"",Compartments!$A101,"")</f>
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="str">
         <f>IF(Compartments!$A102&lt;&gt;"",Compartments!$A102,"")</f>
         <v/>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="str">
         <f>IF(Compartments!$A103&lt;&gt;"",Compartments!$A103,"")</f>
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="str">
         <f>IF(Compartments!$A104&lt;&gt;"",Compartments!$A104,"")</f>
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="str">
         <f>IF(Compartments!$A105&lt;&gt;"",Compartments!$A105,"")</f>
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="str">
         <f>IF(Compartments!$A106&lt;&gt;"",Compartments!$A106,"")</f>
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="str">
         <f>IF(Compartments!$A107&lt;&gt;"",Compartments!$A107,"")</f>
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="str">
         <f>IF(Compartments!$A108&lt;&gt;"",Compartments!$A108,"")</f>
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="str">
         <f>IF(Compartments!$A109&lt;&gt;"",Compartments!$A109,"")</f>
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="str">
         <f>IF(Compartments!$A110&lt;&gt;"",Compartments!$A110,"")</f>
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="str">
         <f>IF(Compartments!$A111&lt;&gt;"",Compartments!$A111,"")</f>
         <v/>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="str">
         <f>IF(Compartments!$A112&lt;&gt;"",Compartments!$A112,"")</f>
         <v/>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="str">
         <f>IF(Compartments!$A113&lt;&gt;"",Compartments!$A113,"")</f>
         <v/>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="str">
         <f>IF(Compartments!$A114&lt;&gt;"",Compartments!$A114,"")</f>
         <v/>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="str">
         <f>IF(Compartments!$A115&lt;&gt;"",Compartments!$A115,"")</f>
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="str">
         <f>IF(Compartments!$A116&lt;&gt;"",Compartments!$A116,"")</f>
         <v/>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="str">
         <f>IF(Compartments!$A117&lt;&gt;"",Compartments!$A117,"")</f>
         <v/>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="str">
         <f>IF(Compartments!$A118&lt;&gt;"",Compartments!$A118,"")</f>
         <v/>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="str">
         <f>IF(Compartments!$A119&lt;&gt;"",Compartments!$A119,"")</f>
         <v/>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="str">
         <f>IF(Compartments!$A120&lt;&gt;"",Compartments!$A120,"")</f>
         <v/>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="str">
         <f>IF(Compartments!$A121&lt;&gt;"",Compartments!$A121,"")</f>
         <v/>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="str">
         <f>IF(Compartments!$A122&lt;&gt;"",Compartments!$A122,"")</f>
         <v/>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="str">
         <f>IF(Compartments!$A123&lt;&gt;"",Compartments!$A123,"")</f>
         <v/>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="str">
         <f>IF(Compartments!$A124&lt;&gt;"",Compartments!$A124,"")</f>
         <v/>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="str">
         <f>IF(Compartments!$A125&lt;&gt;"",Compartments!$A125,"")</f>
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="str">
         <f>IF(Compartments!$A126&lt;&gt;"",Compartments!$A126,"")</f>
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="str">
         <f>IF(Compartments!$A127&lt;&gt;"",Compartments!$A127,"")</f>
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="str">
         <f>IF(Compartments!$A128&lt;&gt;"",Compartments!$A128,"")</f>
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="str">
         <f>IF(Compartments!$A129&lt;&gt;"",Compartments!$A129,"")</f>
         <v/>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="str">
         <f>IF(Compartments!$A130&lt;&gt;"",Compartments!$A130,"")</f>
         <v/>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="str">
         <f>IF(Compartments!$A131&lt;&gt;"",Compartments!$A131,"")</f>
         <v/>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="str">
         <f>IF(Compartments!$A132&lt;&gt;"",Compartments!$A132,"")</f>
         <v/>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="str">
         <f>IF(Compartments!$A133&lt;&gt;"",Compartments!$A133,"")</f>
         <v/>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="str">
         <f>IF(Compartments!$A134&lt;&gt;"",Compartments!$A134,"")</f>
         <v/>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="str">
         <f>IF(Compartments!$A135&lt;&gt;"",Compartments!$A135,"")</f>
         <v/>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="str">
         <f>IF(Compartments!$A136&lt;&gt;"",Compartments!$A136,"")</f>
         <v/>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="str">
         <f>IF(Compartments!$A137&lt;&gt;"",Compartments!$A137,"")</f>
         <v/>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="str">
         <f>IF(Compartments!$A138&lt;&gt;"",Compartments!$A138,"")</f>
         <v/>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="str">
         <f>IF(Compartments!$A139&lt;&gt;"",Compartments!$A139,"")</f>
         <v/>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="str">
         <f>IF(Compartments!$A140&lt;&gt;"",Compartments!$A140,"")</f>
         <v/>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="str">
         <f>IF(Compartments!$A141&lt;&gt;"",Compartments!$A141,"")</f>
         <v/>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="str">
         <f>IF(Compartments!$A142&lt;&gt;"",Compartments!$A142,"")</f>
         <v/>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="str">
         <f>IF(Compartments!$A143&lt;&gt;"",Compartments!$A143,"")</f>
         <v/>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="str">
         <f>IF(Compartments!$A144&lt;&gt;"",Compartments!$A144,"")</f>
         <v/>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="str">
         <f>IF(Compartments!$A145&lt;&gt;"",Compartments!$A145,"")</f>
         <v/>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="str">
         <f>IF(Compartments!$A146&lt;&gt;"",Compartments!$A146,"")</f>
         <v/>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="str">
         <f>IF(Compartments!$A147&lt;&gt;"",Compartments!$A147,"")</f>
         <v/>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="str">
         <f>IF(Compartments!$A148&lt;&gt;"",Compartments!$A148,"")</f>
         <v/>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="str">
         <f>IF(Compartments!$A149&lt;&gt;"",Compartments!$A149,"")</f>
         <v/>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="str">
         <f>IF(Compartments!$A150&lt;&gt;"",Compartments!$A150,"")</f>
         <v/>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="str">
         <f>IF(Compartments!$A151&lt;&gt;"",Compartments!$A151,"")</f>
         <v/>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="str">
         <f>IF(Compartments!$A152&lt;&gt;"",Compartments!$A152,"")</f>
         <v/>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="str">
         <f>IF(Compartments!$A153&lt;&gt;"",Compartments!$A153,"")</f>
         <v/>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" s="3" t="str">
         <f>IF(Compartments!$A154&lt;&gt;"",Compartments!$A154,"")</f>
         <v/>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="str">
         <f>IF(Compartments!$A155&lt;&gt;"",Compartments!$A155,"")</f>
         <v/>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="str">
         <f>IF(Compartments!$A156&lt;&gt;"",Compartments!$A156,"")</f>
         <v/>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="str">
         <f>IF(Compartments!$A157&lt;&gt;"",Compartments!$A157,"")</f>
         <v/>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="str">
         <f>IF(Compartments!$A158&lt;&gt;"",Compartments!$A158,"")</f>
         <v/>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="str">
         <f>IF(Compartments!$A159&lt;&gt;"",Compartments!$A159,"")</f>
         <v/>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" s="3" t="str">
         <f>IF(Compartments!$A160&lt;&gt;"",Compartments!$A160,"")</f>
         <v/>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="str">
         <f>IF(Compartments!$A161&lt;&gt;"",Compartments!$A161,"")</f>
         <v/>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="str">
         <f>IF(Compartments!$A162&lt;&gt;"",Compartments!$A162,"")</f>
         <v/>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="str">
         <f>IF(Compartments!$A163&lt;&gt;"",Compartments!$A163,"")</f>
         <v/>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="str">
         <f>IF(Compartments!$A164&lt;&gt;"",Compartments!$A164,"")</f>
         <v/>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="str">
         <f>IF(Compartments!$A165&lt;&gt;"",Compartments!$A165,"")</f>
         <v/>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="str">
         <f>IF(Compartments!$A166&lt;&gt;"",Compartments!$A166,"")</f>
         <v/>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="str">
         <f>IF(Compartments!$A167&lt;&gt;"",Compartments!$A167,"")</f>
         <v/>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="str">
         <f>IF(Compartments!$A168&lt;&gt;"",Compartments!$A168,"")</f>
         <v/>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="str">
         <f>IF(Compartments!$A169&lt;&gt;"",Compartments!$A169,"")</f>
         <v/>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="str">
         <f>IF(Compartments!$A170&lt;&gt;"",Compartments!$A170,"")</f>
         <v/>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="str">
         <f>IF(Compartments!$A171&lt;&gt;"",Compartments!$A171,"")</f>
         <v/>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="str">
         <f>IF(Compartments!$A172&lt;&gt;"",Compartments!$A172,"")</f>
         <v/>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="str">
         <f>IF(Compartments!$A173&lt;&gt;"",Compartments!$A173,"")</f>
         <v/>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="str">
         <f>IF(Compartments!$A174&lt;&gt;"",Compartments!$A174,"")</f>
         <v/>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="str">
         <f>IF(Compartments!$A175&lt;&gt;"",Compartments!$A175,"")</f>
         <v/>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="str">
         <f>IF(Compartments!$A176&lt;&gt;"",Compartments!$A176,"")</f>
         <v/>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="str">
         <f>IF(Compartments!$A177&lt;&gt;"",Compartments!$A177,"")</f>
         <v/>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" s="3" t="str">
         <f>IF(Compartments!$A178&lt;&gt;"",Compartments!$A178,"")</f>
         <v/>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" s="3" t="str">
         <f>IF(Compartments!$A179&lt;&gt;"",Compartments!$A179,"")</f>
         <v/>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" s="3" t="str">
         <f>IF(Compartments!$A180&lt;&gt;"",Compartments!$A180,"")</f>
         <v/>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="str">
         <f>IF(Compartments!$A181&lt;&gt;"",Compartments!$A181,"")</f>
         <v/>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="str">
         <f>IF(Compartments!$A182&lt;&gt;"",Compartments!$A182,"")</f>
         <v/>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" s="3" t="str">
         <f>IF(Compartments!$A183&lt;&gt;"",Compartments!$A183,"")</f>
         <v/>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" s="3" t="str">
         <f>IF(Compartments!$A184&lt;&gt;"",Compartments!$A184,"")</f>
         <v/>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="str">
         <f>IF(Compartments!$A185&lt;&gt;"",Compartments!$A185,"")</f>
         <v/>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" s="3" t="str">
         <f>IF(Compartments!$A186&lt;&gt;"",Compartments!$A186,"")</f>
         <v/>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="str">
         <f>IF(Compartments!$A187&lt;&gt;"",Compartments!$A187,"")</f>
         <v/>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" s="3" t="str">
         <f>IF(Compartments!$A188&lt;&gt;"",Compartments!$A188,"")</f>
         <v/>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" s="3" t="str">
         <f>IF(Compartments!$A189&lt;&gt;"",Compartments!$A189,"")</f>
         <v/>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" s="3" t="str">
         <f>IF(Compartments!$A190&lt;&gt;"",Compartments!$A190,"")</f>
         <v/>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" s="3" t="str">
         <f>IF(Compartments!$A191&lt;&gt;"",Compartments!$A191,"")</f>
         <v/>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="str">
         <f>IF(Compartments!$A192&lt;&gt;"",Compartments!$A192,"")</f>
         <v/>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="str">
         <f>IF(Compartments!$A193&lt;&gt;"",Compartments!$A193,"")</f>
         <v/>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="str">
         <f>IF(Compartments!$A194&lt;&gt;"",Compartments!$A194,"")</f>
         <v/>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="str">
         <f>IF(Compartments!$A195&lt;&gt;"",Compartments!$A195,"")</f>
         <v/>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="str">
         <f>IF(Compartments!$A196&lt;&gt;"",Compartments!$A196,"")</f>
         <v/>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="str">
         <f>IF(Compartments!$A197&lt;&gt;"",Compartments!$A197,"")</f>
         <v/>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="str">
         <f>IF(Compartments!$A198&lt;&gt;"",Compartments!$A198,"")</f>
         <v/>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="str">
         <f>IF(Compartments!$A199&lt;&gt;"",Compartments!$A199,"")</f>
         <v/>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" s="3" t="str">
         <f>IF(Compartments!$A200&lt;&gt;"",Compartments!$A200,"")</f>
         <v/>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="str">
         <f>IF(Compartments!$A201&lt;&gt;"",Compartments!$A201,"")</f>
         <v/>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="str">
         <f>IF(Compartments!$A202&lt;&gt;"",Compartments!$A202,"")</f>
         <v/>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="str">
         <f>IF(Compartments!$A203&lt;&gt;"",Compartments!$A203,"")</f>
         <v/>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" s="3" t="str">
         <f>IF(Compartments!$A204&lt;&gt;"",Compartments!$A204,"")</f>
         <v/>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="str">
         <f>IF(Compartments!$A205&lt;&gt;"",Compartments!$A205,"")</f>
         <v/>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" s="3" t="str">
         <f>IF(Compartments!$A206&lt;&gt;"",Compartments!$A206,"")</f>
         <v/>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="str">
         <f>IF(Compartments!$A207&lt;&gt;"",Compartments!$A207,"")</f>
         <v/>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="str">
         <f>IF(Compartments!$A208&lt;&gt;"",Compartments!$A208,"")</f>
         <v/>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="str">
         <f>IF(Compartments!$A209&lt;&gt;"",Compartments!$A209,"")</f>
         <v/>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" s="3" t="str">
         <f>IF(Compartments!$A210&lt;&gt;"",Compartments!$A210,"")</f>
         <v/>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="str">
         <f>IF(Compartments!$A211&lt;&gt;"",Compartments!$A211,"")</f>
         <v/>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="str">
         <f>IF(Compartments!$A212&lt;&gt;"",Compartments!$A212,"")</f>
         <v/>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" s="3" t="str">
         <f>IF(Compartments!$A213&lt;&gt;"",Compartments!$A213,"")</f>
         <v/>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" s="3" t="str">
         <f>IF(Compartments!$A214&lt;&gt;"",Compartments!$A214,"")</f>
         <v/>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" s="3" t="str">
         <f>IF(Compartments!$A215&lt;&gt;"",Compartments!$A215,"")</f>
         <v/>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216" s="3" t="str">
         <f>IF(Compartments!$A216&lt;&gt;"",Compartments!$A216,"")</f>
         <v/>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217" s="3" t="str">
         <f>IF(Compartments!$A217&lt;&gt;"",Compartments!$A217,"")</f>
         <v/>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218" s="3" t="str">
         <f>IF(Compartments!$A218&lt;&gt;"",Compartments!$A218,"")</f>
         <v/>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A219" s="3" t="str">
         <f>IF(Compartments!$A219&lt;&gt;"",Compartments!$A219,"")</f>
         <v/>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="str">
         <f>IF(Compartments!$A220&lt;&gt;"",Compartments!$A220,"")</f>
         <v/>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A221" s="3" t="str">
         <f>IF(Compartments!$A221&lt;&gt;"",Compartments!$A221,"")</f>
         <v/>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A222" s="3" t="str">
         <f>IF(Compartments!$A222&lt;&gt;"",Compartments!$A222,"")</f>
         <v/>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A223" s="3" t="str">
         <f>IF(Compartments!$A223&lt;&gt;"",Compartments!$A223,"")</f>
         <v/>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A224" s="3" t="str">
         <f>IF(Compartments!$A224&lt;&gt;"",Compartments!$A224,"")</f>
         <v/>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A225" s="3" t="str">
         <f>IF(Compartments!$A225&lt;&gt;"",Compartments!$A225,"")</f>
         <v/>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A226" s="3" t="str">
         <f>IF(Compartments!$A226&lt;&gt;"",Compartments!$A226,"")</f>
         <v/>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A227" s="3" t="str">
         <f>IF(Compartments!$A227&lt;&gt;"",Compartments!$A227,"")</f>
         <v/>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A228" s="3" t="str">
         <f>IF(Compartments!$A228&lt;&gt;"",Compartments!$A228,"")</f>
         <v/>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A229" s="3" t="str">
         <f>IF(Compartments!$A229&lt;&gt;"",Compartments!$A229,"")</f>
         <v/>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A230" s="3" t="str">
         <f>IF(Compartments!$A230&lt;&gt;"",Compartments!$A230,"")</f>
         <v/>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A231" s="3" t="str">
         <f>IF(Compartments!$A231&lt;&gt;"",Compartments!$A231,"")</f>
         <v/>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A232" s="3" t="str">
         <f>IF(Compartments!$A232&lt;&gt;"",Compartments!$A232,"")</f>
         <v/>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A233" s="3" t="str">
         <f>IF(Compartments!$A233&lt;&gt;"",Compartments!$A233,"")</f>
         <v/>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A234" s="3" t="str">
         <f>IF(Compartments!$A234&lt;&gt;"",Compartments!$A234,"")</f>
         <v/>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A235" s="3" t="str">
         <f>IF(Compartments!$A235&lt;&gt;"",Compartments!$A235,"")</f>
         <v/>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A236" s="3" t="str">
         <f>IF(Compartments!$A236&lt;&gt;"",Compartments!$A236,"")</f>
         <v/>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A237" s="3" t="str">
         <f>IF(Compartments!$A237&lt;&gt;"",Compartments!$A237,"")</f>
         <v/>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A238" s="3" t="str">
         <f>IF(Compartments!$A238&lt;&gt;"",Compartments!$A238,"")</f>
         <v/>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A239" s="3" t="str">
         <f>IF(Compartments!$A239&lt;&gt;"",Compartments!$A239,"")</f>
         <v/>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A240" s="3" t="str">
         <f>IF(Compartments!$A240&lt;&gt;"",Compartments!$A240,"")</f>
         <v/>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A241" s="3" t="str">
         <f>IF(Compartments!$A241&lt;&gt;"",Compartments!$A241,"")</f>
         <v/>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A242" s="3" t="str">
         <f>IF(Compartments!$A242&lt;&gt;"",Compartments!$A242,"")</f>
         <v/>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A243" s="3" t="str">
         <f>IF(Compartments!$A243&lt;&gt;"",Compartments!$A243,"")</f>
         <v/>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A244" s="3" t="str">
         <f>IF(Compartments!$A244&lt;&gt;"",Compartments!$A244,"")</f>
         <v/>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A245" s="3" t="str">
         <f>IF(Compartments!$A245&lt;&gt;"",Compartments!$A245,"")</f>
         <v/>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="str">
         <f>IF(Compartments!$A246&lt;&gt;"",Compartments!$A246,"")</f>
         <v/>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A247" s="3" t="str">
         <f>IF(Compartments!$A247&lt;&gt;"",Compartments!$A247,"")</f>
         <v/>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="str">
         <f>IF(Compartments!$A248&lt;&gt;"",Compartments!$A248,"")</f>
         <v/>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="str">
         <f>IF(Compartments!$A249&lt;&gt;"",Compartments!$A249,"")</f>
         <v/>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="str">
         <f>IF(Compartments!$A250&lt;&gt;"",Compartments!$A250,"")</f>
         <v/>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="str">
         <f>IF(Compartments!$A251&lt;&gt;"",Compartments!$A251,"")</f>
         <v/>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="str">
         <f>IF(Compartments!$A252&lt;&gt;"",Compartments!$A252,"")</f>
         <v/>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="str">
         <f>IF(Compartments!$A253&lt;&gt;"",Compartments!$A253,"")</f>
         <v/>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="str">
         <f>IF(Compartments!$A254&lt;&gt;"",Compartments!$A254,"")</f>
         <v/>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="str">
         <f>IF(Compartments!$A255&lt;&gt;"",Compartments!$A255,"")</f>
         <v/>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="str">
         <f>IF(Compartments!$A256&lt;&gt;"",Compartments!$A256,"")</f>
         <v/>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="str">
         <f>IF(Compartments!$A257&lt;&gt;"",Compartments!$A257,"")</f>
         <v/>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="str">
         <f>IF(Compartments!$A258&lt;&gt;"",Compartments!$A258,"")</f>
         <v/>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="str">
         <f>IF(Compartments!$A259&lt;&gt;"",Compartments!$A259,"")</f>
         <v/>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A260" s="3" t="str">
         <f>IF(Compartments!$A260&lt;&gt;"",Compartments!$A260,"")</f>
         <v/>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="str">
         <f>IF(Compartments!$A261&lt;&gt;"",Compartments!$A261,"")</f>
         <v/>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="str">
         <f>IF(Compartments!$A262&lt;&gt;"",Compartments!$A262,"")</f>
         <v/>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="str">
         <f>IF(Compartments!$A263&lt;&gt;"",Compartments!$A263,"")</f>
         <v/>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A264" s="3" t="str">
         <f>IF(Compartments!$A264&lt;&gt;"",Compartments!$A264,"")</f>
         <v/>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="str">
         <f>IF(Compartments!$A265&lt;&gt;"",Compartments!$A265,"")</f>
         <v/>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A266" s="3" t="str">
         <f>IF(Compartments!$A266&lt;&gt;"",Compartments!$A266,"")</f>
         <v/>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A267" s="3" t="str">
         <f>IF(Compartments!$A267&lt;&gt;"",Compartments!$A267,"")</f>
         <v/>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="str">
         <f>IF(Compartments!$A268&lt;&gt;"",Compartments!$A268,"")</f>
         <v/>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A269" s="3" t="str">
         <f>IF(Compartments!$A269&lt;&gt;"",Compartments!$A269,"")</f>
         <v/>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A270" s="3" t="str">
         <f>IF(Compartments!$A270&lt;&gt;"",Compartments!$A270,"")</f>
         <v/>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A271" s="3" t="str">
         <f>IF(Compartments!$A271&lt;&gt;"",Compartments!$A271,"")</f>
         <v/>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A272" s="3" t="str">
         <f>IF(Compartments!$A272&lt;&gt;"",Compartments!$A272,"")</f>
         <v/>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="str">
         <f>IF(Compartments!$A273&lt;&gt;"",Compartments!$A273,"")</f>
         <v/>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A274" s="3" t="str">
         <f>IF(Compartments!$A274&lt;&gt;"",Compartments!$A274,"")</f>
         <v/>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A275" s="3" t="str">
         <f>IF(Compartments!$A275&lt;&gt;"",Compartments!$A275,"")</f>
         <v/>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A276" s="3" t="str">
         <f>IF(Compartments!$A276&lt;&gt;"",Compartments!$A276,"")</f>
         <v/>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="str">
         <f>IF(Compartments!$A277&lt;&gt;"",Compartments!$A277,"")</f>
         <v/>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A278" s="3" t="str">
         <f>IF(Compartments!$A278&lt;&gt;"",Compartments!$A278,"")</f>
         <v/>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A279" s="3" t="str">
         <f>IF(Compartments!$A279&lt;&gt;"",Compartments!$A279,"")</f>
         <v/>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A280" s="3" t="str">
         <f>IF(Compartments!$A280&lt;&gt;"",Compartments!$A280,"")</f>
         <v/>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="str">
         <f>IF(Compartments!$A281&lt;&gt;"",Compartments!$A281,"")</f>
         <v/>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A282" s="3" t="str">
         <f>IF(Compartments!$A282&lt;&gt;"",Compartments!$A282,"")</f>
         <v/>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="str">
         <f>IF(Compartments!$A283&lt;&gt;"",Compartments!$A283,"")</f>
         <v/>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A284" s="3" t="str">
         <f>IF(Compartments!$A284&lt;&gt;"",Compartments!$A284,"")</f>
         <v/>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A285" s="3" t="str">
         <f>IF(Compartments!$A285&lt;&gt;"",Compartments!$A285,"")</f>
         <v/>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A286" s="3" t="str">
         <f>IF(Compartments!$A286&lt;&gt;"",Compartments!$A286,"")</f>
         <v/>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A287" s="3" t="str">
         <f>IF(Compartments!$A287&lt;&gt;"",Compartments!$A287,"")</f>
         <v/>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A288" s="3" t="str">
         <f>IF(Compartments!$A288&lt;&gt;"",Compartments!$A288,"")</f>
         <v/>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A289" s="3" t="str">
         <f>IF(Compartments!$A289&lt;&gt;"",Compartments!$A289,"")</f>
         <v/>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A290" s="3" t="str">
         <f>IF(Compartments!$A290&lt;&gt;"",Compartments!$A290,"")</f>
         <v/>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A291" s="3" t="str">
         <f>IF(Compartments!$A291&lt;&gt;"",Compartments!$A291,"")</f>
         <v/>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A292" s="3" t="str">
         <f>IF(Compartments!$A292&lt;&gt;"",Compartments!$A292,"")</f>
         <v/>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A293" s="3" t="str">
         <f>IF(Compartments!$A293&lt;&gt;"",Compartments!$A293,"")</f>
         <v/>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A294" s="3" t="str">
         <f>IF(Compartments!$A294&lt;&gt;"",Compartments!$A294,"")</f>
         <v/>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="str">
         <f>IF(Compartments!$A295&lt;&gt;"",Compartments!$A295,"")</f>
         <v/>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A296" s="3" t="str">
         <f>IF(Compartments!$A296&lt;&gt;"",Compartments!$A296,"")</f>
         <v/>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A297" s="3" t="str">
         <f>IF(Compartments!$A297&lt;&gt;"",Compartments!$A297,"")</f>
         <v/>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A298" s="3" t="str">
         <f>IF(Compartments!$A298&lt;&gt;"",Compartments!$A298,"")</f>
         <v/>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A299" s="3" t="str">
         <f>IF(Compartments!$A299&lt;&gt;"",Compartments!$A299,"")</f>
         <v/>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A300" s="3" t="str">
         <f>IF(Compartments!$A300&lt;&gt;"",Compartments!$A300,"")</f>
         <v/>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A301" s="3" t="str">
         <f>IF(Compartments!$A301&lt;&gt;"",Compartments!$A301,"")</f>
         <v/>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A302" s="3" t="str">
         <f>IF(Compartments!$A302&lt;&gt;"",Compartments!$A302,"")</f>
         <v/>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A303" s="3" t="str">
         <f>IF(Compartments!$A303&lt;&gt;"",Compartments!$A303,"")</f>
         <v/>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A304" s="3" t="str">
         <f>IF(Compartments!$A304&lt;&gt;"",Compartments!$A304,"")</f>
         <v/>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A305" s="3" t="str">
         <f>IF(Compartments!$A305&lt;&gt;"",Compartments!$A305,"")</f>
         <v/>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A306" s="3" t="str">
         <f>IF(Compartments!$A306&lt;&gt;"",Compartments!$A306,"")</f>
         <v/>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A307" s="3" t="str">
         <f>IF(Compartments!$A307&lt;&gt;"",Compartments!$A307,"")</f>
         <v/>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A308" s="3" t="str">
         <f>IF(Compartments!$A308&lt;&gt;"",Compartments!$A308,"")</f>
         <v/>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A309" s="3" t="str">
         <f>IF(Compartments!$A309&lt;&gt;"",Compartments!$A309,"")</f>
         <v/>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A310" s="3" t="str">
         <f>IF(Compartments!$A310&lt;&gt;"",Compartments!$A310,"")</f>
         <v/>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A311" s="3" t="str">
         <f>IF(Compartments!$A311&lt;&gt;"",Compartments!$A311,"")</f>
         <v/>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A312" s="3" t="str">
         <f>IF(Compartments!$A312&lt;&gt;"",Compartments!$A312,"")</f>
         <v/>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A313" s="3" t="str">
         <f>IF(Compartments!$A313&lt;&gt;"",Compartments!$A313,"")</f>
         <v/>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A314" s="3" t="str">
         <f>IF(Compartments!$A314&lt;&gt;"",Compartments!$A314,"")</f>
         <v/>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A315" s="3" t="str">
         <f>IF(Compartments!$A315&lt;&gt;"",Compartments!$A315,"")</f>
         <v/>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A316" s="3" t="str">
         <f>IF(Compartments!$A316&lt;&gt;"",Compartments!$A316,"")</f>
         <v/>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A317" s="3" t="str">
         <f>IF(Compartments!$A317&lt;&gt;"",Compartments!$A317,"")</f>
         <v/>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A318" s="3" t="str">
         <f>IF(Compartments!$A318&lt;&gt;"",Compartments!$A318,"")</f>
         <v/>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A319" s="3" t="str">
         <f>IF(Compartments!$A319&lt;&gt;"",Compartments!$A319,"")</f>
         <v/>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A320" s="3" t="str">
         <f>IF(Compartments!$A320&lt;&gt;"",Compartments!$A320,"")</f>
         <v/>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A321" s="3" t="str">
         <f>IF(Compartments!$A321&lt;&gt;"",Compartments!$A321,"")</f>
         <v/>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A322" s="3" t="str">
         <f>IF(Compartments!$A322&lt;&gt;"",Compartments!$A322,"")</f>
         <v/>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A323" s="3" t="str">
         <f>IF(Compartments!$A323&lt;&gt;"",Compartments!$A323,"")</f>
         <v/>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A324" s="3" t="str">
         <f>IF(Compartments!$A324&lt;&gt;"",Compartments!$A324,"")</f>
         <v/>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A325" s="3" t="str">
         <f>IF(Compartments!$A325&lt;&gt;"",Compartments!$A325,"")</f>
         <v/>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A326" s="3" t="str">
         <f>IF(Compartments!$A326&lt;&gt;"",Compartments!$A326,"")</f>
         <v/>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A327" s="3" t="str">
         <f>IF(Compartments!$A327&lt;&gt;"",Compartments!$A327,"")</f>
         <v/>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A328" s="3" t="str">
         <f>IF(Compartments!$A328&lt;&gt;"",Compartments!$A328,"")</f>
         <v/>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A329" s="3" t="str">
         <f>IF(Compartments!$A329&lt;&gt;"",Compartments!$A329,"")</f>
         <v/>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A330" s="3" t="str">
         <f>IF(Compartments!$A330&lt;&gt;"",Compartments!$A330,"")</f>
         <v/>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A331" s="3" t="str">
         <f>IF(Compartments!$A331&lt;&gt;"",Compartments!$A331,"")</f>
         <v/>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A332" s="3" t="str">
         <f>IF(Compartments!$A332&lt;&gt;"",Compartments!$A332,"")</f>
         <v/>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A333" s="3" t="str">
         <f>IF(Compartments!$A333&lt;&gt;"",Compartments!$A333,"")</f>
         <v/>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A334" s="3" t="str">
         <f>IF(Compartments!$A334&lt;&gt;"",Compartments!$A334,"")</f>
         <v/>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A335" s="3" t="str">
         <f>IF(Compartments!$A335&lt;&gt;"",Compartments!$A335,"")</f>
         <v/>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A336" s="3" t="str">
         <f>IF(Compartments!$A336&lt;&gt;"",Compartments!$A336,"")</f>
         <v/>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A337" s="3" t="str">
         <f>IF(Compartments!$A337&lt;&gt;"",Compartments!$A337,"")</f>
         <v/>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A338" s="3" t="str">
         <f>IF(Compartments!$A338&lt;&gt;"",Compartments!$A338,"")</f>
         <v/>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A339" s="3" t="str">
         <f>IF(Compartments!$A339&lt;&gt;"",Compartments!$A339,"")</f>
         <v/>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A340" s="3" t="str">
         <f>IF(Compartments!$A340&lt;&gt;"",Compartments!$A340,"")</f>
         <v/>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A341" s="3" t="str">
         <f>IF(Compartments!$A341&lt;&gt;"",Compartments!$A341,"")</f>
         <v/>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A342" s="3" t="str">
         <f>IF(Compartments!$A342&lt;&gt;"",Compartments!$A342,"")</f>
         <v/>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A343" s="3" t="str">
         <f>IF(Compartments!$A343&lt;&gt;"",Compartments!$A343,"")</f>
         <v/>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A344" s="3" t="str">
         <f>IF(Compartments!$A344&lt;&gt;"",Compartments!$A344,"")</f>
         <v/>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A345" s="3" t="str">
         <f>IF(Compartments!$A345&lt;&gt;"",Compartments!$A345,"")</f>
         <v/>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A346" s="3" t="str">
         <f>IF(Compartments!$A346&lt;&gt;"",Compartments!$A346,"")</f>
         <v/>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A347" s="3" t="str">
         <f>IF(Compartments!$A347&lt;&gt;"",Compartments!$A347,"")</f>
         <v/>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A348" s="3" t="str">
         <f>IF(Compartments!$A348&lt;&gt;"",Compartments!$A348,"")</f>
         <v/>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A349" s="3" t="str">
         <f>IF(Compartments!$A349&lt;&gt;"",Compartments!$A349,"")</f>
         <v/>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A350" s="3" t="str">
         <f>IF(Compartments!$A350&lt;&gt;"",Compartments!$A350,"")</f>
         <v/>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A351" s="3" t="str">
         <f>IF(Compartments!$A351&lt;&gt;"",Compartments!$A351,"")</f>
         <v/>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A352" s="3" t="str">
         <f>IF(Compartments!$A352&lt;&gt;"",Compartments!$A352,"")</f>
         <v/>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A353" s="3" t="str">
         <f>IF(Compartments!$A353&lt;&gt;"",Compartments!$A353,"")</f>
         <v/>
       </c>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A354" s="3" t="str">
         <f>IF(Compartments!$A354&lt;&gt;"",Compartments!$A354,"")</f>
         <v/>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A355" s="3" t="str">
         <f>IF(Compartments!$A355&lt;&gt;"",Compartments!$A355,"")</f>
         <v/>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A356" s="3" t="str">
         <f>IF(Compartments!$A356&lt;&gt;"",Compartments!$A356,"")</f>
         <v/>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A357" s="3" t="str">
         <f>IF(Compartments!$A357&lt;&gt;"",Compartments!$A357,"")</f>
         <v/>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A358" s="3" t="str">
         <f>IF(Compartments!$A358&lt;&gt;"",Compartments!$A358,"")</f>
         <v/>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A359" s="3" t="str">
         <f>IF(Compartments!$A359&lt;&gt;"",Compartments!$A359,"")</f>
         <v/>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A360" s="3" t="str">
         <f>IF(Compartments!$A360&lt;&gt;"",Compartments!$A360,"")</f>
         <v/>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A361" s="3" t="str">
         <f>IF(Compartments!$A361&lt;&gt;"",Compartments!$A361,"")</f>
         <v/>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A362" s="3" t="str">
         <f>IF(Compartments!$A362&lt;&gt;"",Compartments!$A362,"")</f>
         <v/>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A363" s="3" t="str">
         <f>IF(Compartments!$A363&lt;&gt;"",Compartments!$A363,"")</f>
         <v/>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A364" s="3" t="str">
         <f>IF(Compartments!$A364&lt;&gt;"",Compartments!$A364,"")</f>
         <v/>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A365" s="3" t="str">
         <f>IF(Compartments!$A365&lt;&gt;"",Compartments!$A365,"")</f>
         <v/>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A366" s="3" t="str">
         <f>IF(Compartments!$A366&lt;&gt;"",Compartments!$A366,"")</f>
         <v/>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A367" s="3" t="str">
         <f>IF(Compartments!$A367&lt;&gt;"",Compartments!$A367,"")</f>
         <v/>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A368" s="3" t="str">
         <f>IF(Compartments!$A368&lt;&gt;"",Compartments!$A368,"")</f>
         <v/>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A369" s="3" t="str">
         <f>IF(Compartments!$A369&lt;&gt;"",Compartments!$A369,"")</f>
         <v/>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A370" s="3" t="str">
         <f>IF(Compartments!$A370&lt;&gt;"",Compartments!$A370,"")</f>
         <v/>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A371" s="3" t="str">
         <f>IF(Compartments!$A371&lt;&gt;"",Compartments!$A371,"")</f>
         <v/>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A372" s="3" t="str">
         <f>IF(Compartments!$A372&lt;&gt;"",Compartments!$A372,"")</f>
         <v/>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A373" s="3" t="str">
         <f>IF(Compartments!$A373&lt;&gt;"",Compartments!$A373,"")</f>
         <v/>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A374" s="3" t="str">
         <f>IF(Compartments!$A374&lt;&gt;"",Compartments!$A374,"")</f>
         <v/>
       </c>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A375" s="3" t="str">
         <f>IF(Compartments!$A375&lt;&gt;"",Compartments!$A375,"")</f>
         <v/>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A376" s="3" t="str">
         <f>IF(Compartments!$A376&lt;&gt;"",Compartments!$A376,"")</f>
         <v/>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A377" s="3" t="str">
         <f>IF(Compartments!$A377&lt;&gt;"",Compartments!$A377,"")</f>
         <v/>
       </c>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A378" s="3" t="str">
         <f>IF(Compartments!$A378&lt;&gt;"",Compartments!$A378,"")</f>
         <v/>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A379" s="3" t="str">
         <f>IF(Compartments!$A379&lt;&gt;"",Compartments!$A379,"")</f>
         <v/>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A380" s="3" t="str">
         <f>IF(Compartments!$A380&lt;&gt;"",Compartments!$A380,"")</f>
         <v/>
       </c>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A381" s="3" t="str">
         <f>IF(Compartments!$A381&lt;&gt;"",Compartments!$A381,"")</f>
         <v/>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A382" s="3" t="str">
         <f>IF(Compartments!$A382&lt;&gt;"",Compartments!$A382,"")</f>
         <v/>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A383" s="3" t="str">
         <f>IF(Compartments!$A383&lt;&gt;"",Compartments!$A383,"")</f>
         <v/>
       </c>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A384" s="3" t="str">
         <f>IF(Compartments!$A384&lt;&gt;"",Compartments!$A384,"")</f>
         <v/>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A385" s="3" t="str">
         <f>IF(Compartments!$A385&lt;&gt;"",Compartments!$A385,"")</f>
         <v/>
       </c>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A386" s="3" t="str">
         <f>IF(Compartments!$A386&lt;&gt;"",Compartments!$A386,"")</f>
         <v/>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A387" s="3" t="str">
         <f>IF(Compartments!$A387&lt;&gt;"",Compartments!$A387,"")</f>
         <v/>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A388" s="3" t="str">
         <f>IF(Compartments!$A388&lt;&gt;"",Compartments!$A388,"")</f>
         <v/>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A389" s="3" t="str">
         <f>IF(Compartments!$A389&lt;&gt;"",Compartments!$A389,"")</f>
         <v/>
       </c>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A390" s="3" t="str">
         <f>IF(Compartments!$A390&lt;&gt;"",Compartments!$A390,"")</f>
         <v/>
       </c>
     </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A391" s="3" t="str">
         <f>IF(Compartments!$A391&lt;&gt;"",Compartments!$A391,"")</f>
         <v/>
       </c>
     </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A392" s="3" t="str">
         <f>IF(Compartments!$A392&lt;&gt;"",Compartments!$A392,"")</f>
         <v/>
       </c>
     </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A393" s="3" t="str">
         <f>IF(Compartments!$A393&lt;&gt;"",Compartments!$A393,"")</f>
         <v/>
       </c>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A394" s="3" t="str">
         <f>IF(Compartments!$A394&lt;&gt;"",Compartments!$A394,"")</f>
         <v/>
       </c>
     </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A395" s="3" t="str">
         <f>IF(Compartments!$A395&lt;&gt;"",Compartments!$A395,"")</f>
         <v/>
       </c>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A396" s="3" t="str">
         <f>IF(Compartments!$A396&lt;&gt;"",Compartments!$A396,"")</f>
         <v/>
       </c>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A397" s="3" t="str">
         <f>IF(Compartments!$A397&lt;&gt;"",Compartments!$A397,"")</f>
         <v/>
       </c>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A398" s="3" t="str">
         <f>IF(Compartments!$A398&lt;&gt;"",Compartments!$A398,"")</f>
         <v/>
@@ -5306,19 +6037,19 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="6" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="6" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5335,7 +6066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -5344,12 +6075,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>AND(A2&lt;&gt;"",NOT(B2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E1048576">
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="5" priority="8">
       <formula>AND(#REF!&lt;&gt;"",NOT(E2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5375,12 +6106,18 @@
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D0F4671-09BF-4759-B6D1-63C49CDF0760}">
           <x14:formula1>
             <xm:f>'Databook Pages'!$A$2:$A$9999</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E1048576</xm:sqref>
+          <xm:sqref>E2:E1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B08FC4CC-1E7B-E34A-9FEC-BBB85EF18DBD}">
+          <x14:formula1>
+            <xm:f>'[framework_template_advanced.xlsx]Databook Pages'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>E1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5395,51 +6132,51 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" customWidth="1"/>
-    <col min="4" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -5447,22 +6184,27 @@
       <c r="I2" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>AND(A2&lt;&gt;"",NOT(B2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I1048576">
-    <cfRule type="expression" dxfId="1" priority="9">
+    <cfRule type="expression" dxfId="2" priority="10">
       <formula>AND(#REF!&lt;&gt;"",NOT(I2&lt;&gt;""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{7CB7BECB-8CCA-402C-8209-B57AEC65D6EC}">
       <formula1>"n,y"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Code names must be unique" error="Parameter code names must be unique" sqref="A2:A1048576" xr:uid="{E6E68E87-C2E4-4D80-BD6F-D69CE5F2A8E2}">
-      <formula1>COUNTIF(A:A,A2)&lt;2</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Code names must be unique" error="Parameter code names must be unique" sqref="A1:A1048576" xr:uid="{E6E68E87-C2E4-4D80-BD6F-D69CE5F2A8E2}">
+      <formula1>COUNTIF(A:A,A1)&lt;2</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{8BE00A64-F133-4296-8701-DE6AB3B8505B}">
       <formula1>"probability, number, duration, proportion"</formula1>
@@ -5474,7 +6216,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{BE3DBFB1-F6C9-4726-B787-A3DD602656FE}">
+          <x14:cfRule type="expression" priority="2" id="{BE3DBFB1-F6C9-4726-B787-A3DD602656FE}">
             <xm:f>AND(I2&lt;&gt;"",ISERROR(MATCH(I2,'Databook Pages'!$A:$A,0)))</xm:f>
             <x14:dxf>
               <fill>
@@ -5489,12 +6231,18 @@
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B0E7D17F-9C98-4BBD-89E8-B63866BAA65B}">
           <x14:formula1>
             <xm:f>'Databook Pages'!$A$2:$A$9999</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1EB69DA7-5FD8-0D4F-B979-35948680D928}">
+          <x14:formula1>
+            <xm:f>'[framework_template_advanced.xlsx]Databook Pages'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>I1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5506,27 +6254,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45475D22-3C2C-420F-8B01-74A730C6AAB5}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.85546875" customWidth="1"/>
+    <col min="1" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B3" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update template to break links
</commit_message>
<xml_diff>
--- a/atomica/framework_template.xlsx
+++ b/atomica/framework_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/atomica/atomica/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\atomica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{54DEED03-B4C4-E44F-BDB8-5B0CDAB02763}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAC4E37-BDD0-4F1C-A699-CF85B498DE87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -21,7 +21,17 @@
     <sheet name="Parameters" sheetId="6" r:id="rId6"/>
     <sheet name="Cascades" sheetId="10" r:id="rId7"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId8"/>
+  </externalReferences>
   <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1364,14 +1374,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1456,6 +1466,35 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="About"/>
+      <sheetName val="Databook Pages"/>
+      <sheetName val="Compartments"/>
+      <sheetName val="Transitions"/>
+      <sheetName val="Characteristics"/>
+      <sheetName val="Parameters"/>
+      <sheetName val="Interactions"/>
+      <sheetName val="Cascades"/>
+      <sheetName val="Plots"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1784,17 +1823,15 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="97.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="97.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -1802,7 +1839,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="234.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="234.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -1810,22 +1847,22 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1833,7 +1870,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1841,7 +1878,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1849,7 +1886,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1857,7 +1894,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1865,7 +1902,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1887,16 +1924,16 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1904,7 +1941,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1912,7 +1949,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1942,15 +1979,15 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -1963,7 +2000,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -2024,12 +2061,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:398" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:398" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -3622,2383 +3659,2383 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:398" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
         <f>IF(Compartments!$A2&lt;&gt;"",Compartments!$A2,"")</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:398" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f>IF(Compartments!$A3&lt;&gt;"",Compartments!$A3,"")</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:398" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f>IF(Compartments!$A4&lt;&gt;"",Compartments!$A4,"")</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:398" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f>IF(Compartments!$A5&lt;&gt;"",Compartments!$A5,"")</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:398" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f>IF(Compartments!$A6&lt;&gt;"",Compartments!$A6,"")</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:398" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f>IF(Compartments!$A7&lt;&gt;"",Compartments!$A7,"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:398" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f>IF(Compartments!$A8&lt;&gt;"",Compartments!$A8,"")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:398" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str">
         <f>IF(Compartments!$A9&lt;&gt;"",Compartments!$A9,"")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:398" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="str">
         <f>IF(Compartments!$A10&lt;&gt;"",Compartments!$A10,"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:398" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="str">
         <f>IF(Compartments!$A11&lt;&gt;"",Compartments!$A11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:398" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="str">
         <f>IF(Compartments!$A12&lt;&gt;"",Compartments!$A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:398" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="str">
         <f>IF(Compartments!$A13&lt;&gt;"",Compartments!$A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:398" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="str">
         <f>IF(Compartments!$A14&lt;&gt;"",Compartments!$A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:398" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="str">
         <f>IF(Compartments!$A15&lt;&gt;"",Compartments!$A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:398" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="str">
         <f>IF(Compartments!$A16&lt;&gt;"",Compartments!$A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="str">
         <f>IF(Compartments!$A17&lt;&gt;"",Compartments!$A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="str">
         <f>IF(Compartments!$A18&lt;&gt;"",Compartments!$A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="str">
         <f>IF(Compartments!$A19&lt;&gt;"",Compartments!$A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="str">
         <f>IF(Compartments!$A20&lt;&gt;"",Compartments!$A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="str">
         <f>IF(Compartments!$A21&lt;&gt;"",Compartments!$A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="str">
         <f>IF(Compartments!$A22&lt;&gt;"",Compartments!$A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="str">
         <f>IF(Compartments!$A23&lt;&gt;"",Compartments!$A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="str">
         <f>IF(Compartments!$A24&lt;&gt;"",Compartments!$A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="str">
         <f>IF(Compartments!$A25&lt;&gt;"",Compartments!$A25,"")</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="str">
         <f>IF(Compartments!$A26&lt;&gt;"",Compartments!$A26,"")</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="str">
         <f>IF(Compartments!$A27&lt;&gt;"",Compartments!$A27,"")</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="str">
         <f>IF(Compartments!$A28&lt;&gt;"",Compartments!$A28,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="str">
         <f>IF(Compartments!$A29&lt;&gt;"",Compartments!$A29,"")</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="str">
         <f>IF(Compartments!$A30&lt;&gt;"",Compartments!$A30,"")</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="str">
         <f>IF(Compartments!$A31&lt;&gt;"",Compartments!$A31,"")</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="str">
         <f>IF(Compartments!$A32&lt;&gt;"",Compartments!$A32,"")</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="str">
         <f>IF(Compartments!$A33&lt;&gt;"",Compartments!$A33,"")</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="str">
         <f>IF(Compartments!$A34&lt;&gt;"",Compartments!$A34,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="str">
         <f>IF(Compartments!$A35&lt;&gt;"",Compartments!$A35,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="str">
         <f>IF(Compartments!$A36&lt;&gt;"",Compartments!$A36,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="str">
         <f>IF(Compartments!$A37&lt;&gt;"",Compartments!$A37,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="str">
         <f>IF(Compartments!$A38&lt;&gt;"",Compartments!$A38,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="str">
         <f>IF(Compartments!$A39&lt;&gt;"",Compartments!$A39,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="str">
         <f>IF(Compartments!$A40&lt;&gt;"",Compartments!$A40,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="str">
         <f>IF(Compartments!$A41&lt;&gt;"",Compartments!$A41,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="str">
         <f>IF(Compartments!$A42&lt;&gt;"",Compartments!$A42,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="str">
         <f>IF(Compartments!$A43&lt;&gt;"",Compartments!$A43,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="str">
         <f>IF(Compartments!$A44&lt;&gt;"",Compartments!$A44,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="str">
         <f>IF(Compartments!$A45&lt;&gt;"",Compartments!$A45,"")</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="str">
         <f>IF(Compartments!$A46&lt;&gt;"",Compartments!$A46,"")</f>
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="str">
         <f>IF(Compartments!$A47&lt;&gt;"",Compartments!$A47,"")</f>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="str">
         <f>IF(Compartments!$A48&lt;&gt;"",Compartments!$A48,"")</f>
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="str">
         <f>IF(Compartments!$A49&lt;&gt;"",Compartments!$A49,"")</f>
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="str">
         <f>IF(Compartments!$A50&lt;&gt;"",Compartments!$A50,"")</f>
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="str">
         <f>IF(Compartments!$A51&lt;&gt;"",Compartments!$A51,"")</f>
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="str">
         <f>IF(Compartments!$A52&lt;&gt;"",Compartments!$A52,"")</f>
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="str">
         <f>IF(Compartments!$A53&lt;&gt;"",Compartments!$A53,"")</f>
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="str">
         <f>IF(Compartments!$A54&lt;&gt;"",Compartments!$A54,"")</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="str">
         <f>IF(Compartments!$A55&lt;&gt;"",Compartments!$A55,"")</f>
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="str">
         <f>IF(Compartments!$A56&lt;&gt;"",Compartments!$A56,"")</f>
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="str">
         <f>IF(Compartments!$A57&lt;&gt;"",Compartments!$A57,"")</f>
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="str">
         <f>IF(Compartments!$A58&lt;&gt;"",Compartments!$A58,"")</f>
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="str">
         <f>IF(Compartments!$A59&lt;&gt;"",Compartments!$A59,"")</f>
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="str">
         <f>IF(Compartments!$A60&lt;&gt;"",Compartments!$A60,"")</f>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="str">
         <f>IF(Compartments!$A61&lt;&gt;"",Compartments!$A61,"")</f>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="str">
         <f>IF(Compartments!$A62&lt;&gt;"",Compartments!$A62,"")</f>
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="str">
         <f>IF(Compartments!$A63&lt;&gt;"",Compartments!$A63,"")</f>
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="str">
         <f>IF(Compartments!$A64&lt;&gt;"",Compartments!$A64,"")</f>
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="str">
         <f>IF(Compartments!$A65&lt;&gt;"",Compartments!$A65,"")</f>
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="str">
         <f>IF(Compartments!$A66&lt;&gt;"",Compartments!$A66,"")</f>
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="str">
         <f>IF(Compartments!$A67&lt;&gt;"",Compartments!$A67,"")</f>
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="str">
         <f>IF(Compartments!$A68&lt;&gt;"",Compartments!$A68,"")</f>
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="str">
         <f>IF(Compartments!$A69&lt;&gt;"",Compartments!$A69,"")</f>
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="str">
         <f>IF(Compartments!$A70&lt;&gt;"",Compartments!$A70,"")</f>
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="str">
         <f>IF(Compartments!$A71&lt;&gt;"",Compartments!$A71,"")</f>
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="str">
         <f>IF(Compartments!$A72&lt;&gt;"",Compartments!$A72,"")</f>
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="str">
         <f>IF(Compartments!$A73&lt;&gt;"",Compartments!$A73,"")</f>
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="str">
         <f>IF(Compartments!$A74&lt;&gt;"",Compartments!$A74,"")</f>
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="str">
         <f>IF(Compartments!$A75&lt;&gt;"",Compartments!$A75,"")</f>
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="str">
         <f>IF(Compartments!$A76&lt;&gt;"",Compartments!$A76,"")</f>
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="str">
         <f>IF(Compartments!$A77&lt;&gt;"",Compartments!$A77,"")</f>
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="str">
         <f>IF(Compartments!$A78&lt;&gt;"",Compartments!$A78,"")</f>
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="str">
         <f>IF(Compartments!$A79&lt;&gt;"",Compartments!$A79,"")</f>
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="str">
         <f>IF(Compartments!$A80&lt;&gt;"",Compartments!$A80,"")</f>
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="str">
         <f>IF(Compartments!$A81&lt;&gt;"",Compartments!$A81,"")</f>
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="str">
         <f>IF(Compartments!$A82&lt;&gt;"",Compartments!$A82,"")</f>
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="str">
         <f>IF(Compartments!$A83&lt;&gt;"",Compartments!$A83,"")</f>
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="str">
         <f>IF(Compartments!$A84&lt;&gt;"",Compartments!$A84,"")</f>
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="str">
         <f>IF(Compartments!$A85&lt;&gt;"",Compartments!$A85,"")</f>
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="str">
         <f>IF(Compartments!$A86&lt;&gt;"",Compartments!$A86,"")</f>
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="str">
         <f>IF(Compartments!$A87&lt;&gt;"",Compartments!$A87,"")</f>
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="str">
         <f>IF(Compartments!$A88&lt;&gt;"",Compartments!$A88,"")</f>
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="str">
         <f>IF(Compartments!$A89&lt;&gt;"",Compartments!$A89,"")</f>
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="str">
         <f>IF(Compartments!$A90&lt;&gt;"",Compartments!$A90,"")</f>
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="str">
         <f>IF(Compartments!$A91&lt;&gt;"",Compartments!$A91,"")</f>
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="str">
         <f>IF(Compartments!$A92&lt;&gt;"",Compartments!$A92,"")</f>
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="str">
         <f>IF(Compartments!$A93&lt;&gt;"",Compartments!$A93,"")</f>
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="str">
         <f>IF(Compartments!$A94&lt;&gt;"",Compartments!$A94,"")</f>
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="str">
         <f>IF(Compartments!$A95&lt;&gt;"",Compartments!$A95,"")</f>
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="str">
         <f>IF(Compartments!$A96&lt;&gt;"",Compartments!$A96,"")</f>
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="str">
         <f>IF(Compartments!$A97&lt;&gt;"",Compartments!$A97,"")</f>
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="str">
         <f>IF(Compartments!$A98&lt;&gt;"",Compartments!$A98,"")</f>
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="str">
         <f>IF(Compartments!$A99&lt;&gt;"",Compartments!$A99,"")</f>
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="str">
         <f>IF(Compartments!$A100&lt;&gt;"",Compartments!$A100,"")</f>
         <v/>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="str">
         <f>IF(Compartments!$A101&lt;&gt;"",Compartments!$A101,"")</f>
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="str">
         <f>IF(Compartments!$A102&lt;&gt;"",Compartments!$A102,"")</f>
         <v/>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="str">
         <f>IF(Compartments!$A103&lt;&gt;"",Compartments!$A103,"")</f>
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="str">
         <f>IF(Compartments!$A104&lt;&gt;"",Compartments!$A104,"")</f>
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="str">
         <f>IF(Compartments!$A105&lt;&gt;"",Compartments!$A105,"")</f>
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="str">
         <f>IF(Compartments!$A106&lt;&gt;"",Compartments!$A106,"")</f>
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="str">
         <f>IF(Compartments!$A107&lt;&gt;"",Compartments!$A107,"")</f>
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="str">
         <f>IF(Compartments!$A108&lt;&gt;"",Compartments!$A108,"")</f>
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="str">
         <f>IF(Compartments!$A109&lt;&gt;"",Compartments!$A109,"")</f>
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="str">
         <f>IF(Compartments!$A110&lt;&gt;"",Compartments!$A110,"")</f>
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="str">
         <f>IF(Compartments!$A111&lt;&gt;"",Compartments!$A111,"")</f>
         <v/>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="str">
         <f>IF(Compartments!$A112&lt;&gt;"",Compartments!$A112,"")</f>
         <v/>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="str">
         <f>IF(Compartments!$A113&lt;&gt;"",Compartments!$A113,"")</f>
         <v/>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="str">
         <f>IF(Compartments!$A114&lt;&gt;"",Compartments!$A114,"")</f>
         <v/>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="str">
         <f>IF(Compartments!$A115&lt;&gt;"",Compartments!$A115,"")</f>
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="str">
         <f>IF(Compartments!$A116&lt;&gt;"",Compartments!$A116,"")</f>
         <v/>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="str">
         <f>IF(Compartments!$A117&lt;&gt;"",Compartments!$A117,"")</f>
         <v/>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="str">
         <f>IF(Compartments!$A118&lt;&gt;"",Compartments!$A118,"")</f>
         <v/>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="str">
         <f>IF(Compartments!$A119&lt;&gt;"",Compartments!$A119,"")</f>
         <v/>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="str">
         <f>IF(Compartments!$A120&lt;&gt;"",Compartments!$A120,"")</f>
         <v/>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="str">
         <f>IF(Compartments!$A121&lt;&gt;"",Compartments!$A121,"")</f>
         <v/>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="str">
         <f>IF(Compartments!$A122&lt;&gt;"",Compartments!$A122,"")</f>
         <v/>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="str">
         <f>IF(Compartments!$A123&lt;&gt;"",Compartments!$A123,"")</f>
         <v/>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="str">
         <f>IF(Compartments!$A124&lt;&gt;"",Compartments!$A124,"")</f>
         <v/>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="str">
         <f>IF(Compartments!$A125&lt;&gt;"",Compartments!$A125,"")</f>
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="str">
         <f>IF(Compartments!$A126&lt;&gt;"",Compartments!$A126,"")</f>
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="str">
         <f>IF(Compartments!$A127&lt;&gt;"",Compartments!$A127,"")</f>
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="str">
         <f>IF(Compartments!$A128&lt;&gt;"",Compartments!$A128,"")</f>
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="str">
         <f>IF(Compartments!$A129&lt;&gt;"",Compartments!$A129,"")</f>
         <v/>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="str">
         <f>IF(Compartments!$A130&lt;&gt;"",Compartments!$A130,"")</f>
         <v/>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="str">
         <f>IF(Compartments!$A131&lt;&gt;"",Compartments!$A131,"")</f>
         <v/>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="str">
         <f>IF(Compartments!$A132&lt;&gt;"",Compartments!$A132,"")</f>
         <v/>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="str">
         <f>IF(Compartments!$A133&lt;&gt;"",Compartments!$A133,"")</f>
         <v/>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="str">
         <f>IF(Compartments!$A134&lt;&gt;"",Compartments!$A134,"")</f>
         <v/>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="str">
         <f>IF(Compartments!$A135&lt;&gt;"",Compartments!$A135,"")</f>
         <v/>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="str">
         <f>IF(Compartments!$A136&lt;&gt;"",Compartments!$A136,"")</f>
         <v/>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="str">
         <f>IF(Compartments!$A137&lt;&gt;"",Compartments!$A137,"")</f>
         <v/>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="str">
         <f>IF(Compartments!$A138&lt;&gt;"",Compartments!$A138,"")</f>
         <v/>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="str">
         <f>IF(Compartments!$A139&lt;&gt;"",Compartments!$A139,"")</f>
         <v/>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="str">
         <f>IF(Compartments!$A140&lt;&gt;"",Compartments!$A140,"")</f>
         <v/>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="str">
         <f>IF(Compartments!$A141&lt;&gt;"",Compartments!$A141,"")</f>
         <v/>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="str">
         <f>IF(Compartments!$A142&lt;&gt;"",Compartments!$A142,"")</f>
         <v/>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="str">
         <f>IF(Compartments!$A143&lt;&gt;"",Compartments!$A143,"")</f>
         <v/>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="str">
         <f>IF(Compartments!$A144&lt;&gt;"",Compartments!$A144,"")</f>
         <v/>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="str">
         <f>IF(Compartments!$A145&lt;&gt;"",Compartments!$A145,"")</f>
         <v/>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="str">
         <f>IF(Compartments!$A146&lt;&gt;"",Compartments!$A146,"")</f>
         <v/>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="str">
         <f>IF(Compartments!$A147&lt;&gt;"",Compartments!$A147,"")</f>
         <v/>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="str">
         <f>IF(Compartments!$A148&lt;&gt;"",Compartments!$A148,"")</f>
         <v/>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="str">
         <f>IF(Compartments!$A149&lt;&gt;"",Compartments!$A149,"")</f>
         <v/>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="str">
         <f>IF(Compartments!$A150&lt;&gt;"",Compartments!$A150,"")</f>
         <v/>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="str">
         <f>IF(Compartments!$A151&lt;&gt;"",Compartments!$A151,"")</f>
         <v/>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="str">
         <f>IF(Compartments!$A152&lt;&gt;"",Compartments!$A152,"")</f>
         <v/>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="str">
         <f>IF(Compartments!$A153&lt;&gt;"",Compartments!$A153,"")</f>
         <v/>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="str">
         <f>IF(Compartments!$A154&lt;&gt;"",Compartments!$A154,"")</f>
         <v/>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="str">
         <f>IF(Compartments!$A155&lt;&gt;"",Compartments!$A155,"")</f>
         <v/>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="str">
         <f>IF(Compartments!$A156&lt;&gt;"",Compartments!$A156,"")</f>
         <v/>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="str">
         <f>IF(Compartments!$A157&lt;&gt;"",Compartments!$A157,"")</f>
         <v/>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="str">
         <f>IF(Compartments!$A158&lt;&gt;"",Compartments!$A158,"")</f>
         <v/>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="str">
         <f>IF(Compartments!$A159&lt;&gt;"",Compartments!$A159,"")</f>
         <v/>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="str">
         <f>IF(Compartments!$A160&lt;&gt;"",Compartments!$A160,"")</f>
         <v/>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="str">
         <f>IF(Compartments!$A161&lt;&gt;"",Compartments!$A161,"")</f>
         <v/>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="str">
         <f>IF(Compartments!$A162&lt;&gt;"",Compartments!$A162,"")</f>
         <v/>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="str">
         <f>IF(Compartments!$A163&lt;&gt;"",Compartments!$A163,"")</f>
         <v/>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="str">
         <f>IF(Compartments!$A164&lt;&gt;"",Compartments!$A164,"")</f>
         <v/>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="str">
         <f>IF(Compartments!$A165&lt;&gt;"",Compartments!$A165,"")</f>
         <v/>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="str">
         <f>IF(Compartments!$A166&lt;&gt;"",Compartments!$A166,"")</f>
         <v/>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="str">
         <f>IF(Compartments!$A167&lt;&gt;"",Compartments!$A167,"")</f>
         <v/>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="str">
         <f>IF(Compartments!$A168&lt;&gt;"",Compartments!$A168,"")</f>
         <v/>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="str">
         <f>IF(Compartments!$A169&lt;&gt;"",Compartments!$A169,"")</f>
         <v/>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="str">
         <f>IF(Compartments!$A170&lt;&gt;"",Compartments!$A170,"")</f>
         <v/>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="str">
         <f>IF(Compartments!$A171&lt;&gt;"",Compartments!$A171,"")</f>
         <v/>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="str">
         <f>IF(Compartments!$A172&lt;&gt;"",Compartments!$A172,"")</f>
         <v/>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="str">
         <f>IF(Compartments!$A173&lt;&gt;"",Compartments!$A173,"")</f>
         <v/>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="str">
         <f>IF(Compartments!$A174&lt;&gt;"",Compartments!$A174,"")</f>
         <v/>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="str">
         <f>IF(Compartments!$A175&lt;&gt;"",Compartments!$A175,"")</f>
         <v/>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="str">
         <f>IF(Compartments!$A176&lt;&gt;"",Compartments!$A176,"")</f>
         <v/>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="str">
         <f>IF(Compartments!$A177&lt;&gt;"",Compartments!$A177,"")</f>
         <v/>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="str">
         <f>IF(Compartments!$A178&lt;&gt;"",Compartments!$A178,"")</f>
         <v/>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="str">
         <f>IF(Compartments!$A179&lt;&gt;"",Compartments!$A179,"")</f>
         <v/>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="str">
         <f>IF(Compartments!$A180&lt;&gt;"",Compartments!$A180,"")</f>
         <v/>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="str">
         <f>IF(Compartments!$A181&lt;&gt;"",Compartments!$A181,"")</f>
         <v/>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="str">
         <f>IF(Compartments!$A182&lt;&gt;"",Compartments!$A182,"")</f>
         <v/>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="str">
         <f>IF(Compartments!$A183&lt;&gt;"",Compartments!$A183,"")</f>
         <v/>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="str">
         <f>IF(Compartments!$A184&lt;&gt;"",Compartments!$A184,"")</f>
         <v/>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="str">
         <f>IF(Compartments!$A185&lt;&gt;"",Compartments!$A185,"")</f>
         <v/>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="str">
         <f>IF(Compartments!$A186&lt;&gt;"",Compartments!$A186,"")</f>
         <v/>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="str">
         <f>IF(Compartments!$A187&lt;&gt;"",Compartments!$A187,"")</f>
         <v/>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="str">
         <f>IF(Compartments!$A188&lt;&gt;"",Compartments!$A188,"")</f>
         <v/>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="str">
         <f>IF(Compartments!$A189&lt;&gt;"",Compartments!$A189,"")</f>
         <v/>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="str">
         <f>IF(Compartments!$A190&lt;&gt;"",Compartments!$A190,"")</f>
         <v/>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="str">
         <f>IF(Compartments!$A191&lt;&gt;"",Compartments!$A191,"")</f>
         <v/>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="str">
         <f>IF(Compartments!$A192&lt;&gt;"",Compartments!$A192,"")</f>
         <v/>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="str">
         <f>IF(Compartments!$A193&lt;&gt;"",Compartments!$A193,"")</f>
         <v/>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="str">
         <f>IF(Compartments!$A194&lt;&gt;"",Compartments!$A194,"")</f>
         <v/>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="str">
         <f>IF(Compartments!$A195&lt;&gt;"",Compartments!$A195,"")</f>
         <v/>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="str">
         <f>IF(Compartments!$A196&lt;&gt;"",Compartments!$A196,"")</f>
         <v/>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="str">
         <f>IF(Compartments!$A197&lt;&gt;"",Compartments!$A197,"")</f>
         <v/>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="str">
         <f>IF(Compartments!$A198&lt;&gt;"",Compartments!$A198,"")</f>
         <v/>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="str">
         <f>IF(Compartments!$A199&lt;&gt;"",Compartments!$A199,"")</f>
         <v/>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="str">
         <f>IF(Compartments!$A200&lt;&gt;"",Compartments!$A200,"")</f>
         <v/>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="str">
         <f>IF(Compartments!$A201&lt;&gt;"",Compartments!$A201,"")</f>
         <v/>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="str">
         <f>IF(Compartments!$A202&lt;&gt;"",Compartments!$A202,"")</f>
         <v/>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="str">
         <f>IF(Compartments!$A203&lt;&gt;"",Compartments!$A203,"")</f>
         <v/>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="str">
         <f>IF(Compartments!$A204&lt;&gt;"",Compartments!$A204,"")</f>
         <v/>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="str">
         <f>IF(Compartments!$A205&lt;&gt;"",Compartments!$A205,"")</f>
         <v/>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="str">
         <f>IF(Compartments!$A206&lt;&gt;"",Compartments!$A206,"")</f>
         <v/>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="str">
         <f>IF(Compartments!$A207&lt;&gt;"",Compartments!$A207,"")</f>
         <v/>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="str">
         <f>IF(Compartments!$A208&lt;&gt;"",Compartments!$A208,"")</f>
         <v/>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="str">
         <f>IF(Compartments!$A209&lt;&gt;"",Compartments!$A209,"")</f>
         <v/>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="str">
         <f>IF(Compartments!$A210&lt;&gt;"",Compartments!$A210,"")</f>
         <v/>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="str">
         <f>IF(Compartments!$A211&lt;&gt;"",Compartments!$A211,"")</f>
         <v/>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="str">
         <f>IF(Compartments!$A212&lt;&gt;"",Compartments!$A212,"")</f>
         <v/>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="str">
         <f>IF(Compartments!$A213&lt;&gt;"",Compartments!$A213,"")</f>
         <v/>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="str">
         <f>IF(Compartments!$A214&lt;&gt;"",Compartments!$A214,"")</f>
         <v/>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="str">
         <f>IF(Compartments!$A215&lt;&gt;"",Compartments!$A215,"")</f>
         <v/>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="str">
         <f>IF(Compartments!$A216&lt;&gt;"",Compartments!$A216,"")</f>
         <v/>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="str">
         <f>IF(Compartments!$A217&lt;&gt;"",Compartments!$A217,"")</f>
         <v/>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="str">
         <f>IF(Compartments!$A218&lt;&gt;"",Compartments!$A218,"")</f>
         <v/>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="str">
         <f>IF(Compartments!$A219&lt;&gt;"",Compartments!$A219,"")</f>
         <v/>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="str">
         <f>IF(Compartments!$A220&lt;&gt;"",Compartments!$A220,"")</f>
         <v/>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="str">
         <f>IF(Compartments!$A221&lt;&gt;"",Compartments!$A221,"")</f>
         <v/>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="str">
         <f>IF(Compartments!$A222&lt;&gt;"",Compartments!$A222,"")</f>
         <v/>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="str">
         <f>IF(Compartments!$A223&lt;&gt;"",Compartments!$A223,"")</f>
         <v/>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="str">
         <f>IF(Compartments!$A224&lt;&gt;"",Compartments!$A224,"")</f>
         <v/>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="str">
         <f>IF(Compartments!$A225&lt;&gt;"",Compartments!$A225,"")</f>
         <v/>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="str">
         <f>IF(Compartments!$A226&lt;&gt;"",Compartments!$A226,"")</f>
         <v/>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="str">
         <f>IF(Compartments!$A227&lt;&gt;"",Compartments!$A227,"")</f>
         <v/>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="str">
         <f>IF(Compartments!$A228&lt;&gt;"",Compartments!$A228,"")</f>
         <v/>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="str">
         <f>IF(Compartments!$A229&lt;&gt;"",Compartments!$A229,"")</f>
         <v/>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="str">
         <f>IF(Compartments!$A230&lt;&gt;"",Compartments!$A230,"")</f>
         <v/>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="str">
         <f>IF(Compartments!$A231&lt;&gt;"",Compartments!$A231,"")</f>
         <v/>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="str">
         <f>IF(Compartments!$A232&lt;&gt;"",Compartments!$A232,"")</f>
         <v/>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="str">
         <f>IF(Compartments!$A233&lt;&gt;"",Compartments!$A233,"")</f>
         <v/>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="str">
         <f>IF(Compartments!$A234&lt;&gt;"",Compartments!$A234,"")</f>
         <v/>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="str">
         <f>IF(Compartments!$A235&lt;&gt;"",Compartments!$A235,"")</f>
         <v/>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" s="3" t="str">
         <f>IF(Compartments!$A236&lt;&gt;"",Compartments!$A236,"")</f>
         <v/>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="str">
         <f>IF(Compartments!$A237&lt;&gt;"",Compartments!$A237,"")</f>
         <v/>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" s="3" t="str">
         <f>IF(Compartments!$A238&lt;&gt;"",Compartments!$A238,"")</f>
         <v/>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" s="3" t="str">
         <f>IF(Compartments!$A239&lt;&gt;"",Compartments!$A239,"")</f>
         <v/>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" s="3" t="str">
         <f>IF(Compartments!$A240&lt;&gt;"",Compartments!$A240,"")</f>
         <v/>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" s="3" t="str">
         <f>IF(Compartments!$A241&lt;&gt;"",Compartments!$A241,"")</f>
         <v/>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="str">
         <f>IF(Compartments!$A242&lt;&gt;"",Compartments!$A242,"")</f>
         <v/>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" s="3" t="str">
         <f>IF(Compartments!$A243&lt;&gt;"",Compartments!$A243,"")</f>
         <v/>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" s="3" t="str">
         <f>IF(Compartments!$A244&lt;&gt;"",Compartments!$A244,"")</f>
         <v/>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" s="3" t="str">
         <f>IF(Compartments!$A245&lt;&gt;"",Compartments!$A245,"")</f>
         <v/>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246" s="3" t="str">
         <f>IF(Compartments!$A246&lt;&gt;"",Compartments!$A246,"")</f>
         <v/>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" s="3" t="str">
         <f>IF(Compartments!$A247&lt;&gt;"",Compartments!$A247,"")</f>
         <v/>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" s="3" t="str">
         <f>IF(Compartments!$A248&lt;&gt;"",Compartments!$A248,"")</f>
         <v/>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" s="3" t="str">
         <f>IF(Compartments!$A249&lt;&gt;"",Compartments!$A249,"")</f>
         <v/>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" s="3" t="str">
         <f>IF(Compartments!$A250&lt;&gt;"",Compartments!$A250,"")</f>
         <v/>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" s="3" t="str">
         <f>IF(Compartments!$A251&lt;&gt;"",Compartments!$A251,"")</f>
         <v/>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" s="3" t="str">
         <f>IF(Compartments!$A252&lt;&gt;"",Compartments!$A252,"")</f>
         <v/>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" s="3" t="str">
         <f>IF(Compartments!$A253&lt;&gt;"",Compartments!$A253,"")</f>
         <v/>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" s="3" t="str">
         <f>IF(Compartments!$A254&lt;&gt;"",Compartments!$A254,"")</f>
         <v/>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255" s="3" t="str">
         <f>IF(Compartments!$A255&lt;&gt;"",Compartments!$A255,"")</f>
         <v/>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" s="3" t="str">
         <f>IF(Compartments!$A256&lt;&gt;"",Compartments!$A256,"")</f>
         <v/>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" s="3" t="str">
         <f>IF(Compartments!$A257&lt;&gt;"",Compartments!$A257,"")</f>
         <v/>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" s="3" t="str">
         <f>IF(Compartments!$A258&lt;&gt;"",Compartments!$A258,"")</f>
         <v/>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" s="3" t="str">
         <f>IF(Compartments!$A259&lt;&gt;"",Compartments!$A259,"")</f>
         <v/>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" s="3" t="str">
         <f>IF(Compartments!$A260&lt;&gt;"",Compartments!$A260,"")</f>
         <v/>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" s="3" t="str">
         <f>IF(Compartments!$A261&lt;&gt;"",Compartments!$A261,"")</f>
         <v/>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" s="3" t="str">
         <f>IF(Compartments!$A262&lt;&gt;"",Compartments!$A262,"")</f>
         <v/>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" s="3" t="str">
         <f>IF(Compartments!$A263&lt;&gt;"",Compartments!$A263,"")</f>
         <v/>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" s="3" t="str">
         <f>IF(Compartments!$A264&lt;&gt;"",Compartments!$A264,"")</f>
         <v/>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" s="3" t="str">
         <f>IF(Compartments!$A265&lt;&gt;"",Compartments!$A265,"")</f>
         <v/>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" s="3" t="str">
         <f>IF(Compartments!$A266&lt;&gt;"",Compartments!$A266,"")</f>
         <v/>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" s="3" t="str">
         <f>IF(Compartments!$A267&lt;&gt;"",Compartments!$A267,"")</f>
         <v/>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" s="3" t="str">
         <f>IF(Compartments!$A268&lt;&gt;"",Compartments!$A268,"")</f>
         <v/>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" s="3" t="str">
         <f>IF(Compartments!$A269&lt;&gt;"",Compartments!$A269,"")</f>
         <v/>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" s="3" t="str">
         <f>IF(Compartments!$A270&lt;&gt;"",Compartments!$A270,"")</f>
         <v/>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" s="3" t="str">
         <f>IF(Compartments!$A271&lt;&gt;"",Compartments!$A271,"")</f>
         <v/>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" s="3" t="str">
         <f>IF(Compartments!$A272&lt;&gt;"",Compartments!$A272,"")</f>
         <v/>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" s="3" t="str">
         <f>IF(Compartments!$A273&lt;&gt;"",Compartments!$A273,"")</f>
         <v/>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" s="3" t="str">
         <f>IF(Compartments!$A274&lt;&gt;"",Compartments!$A274,"")</f>
         <v/>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" s="3" t="str">
         <f>IF(Compartments!$A275&lt;&gt;"",Compartments!$A275,"")</f>
         <v/>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" s="3" t="str">
         <f>IF(Compartments!$A276&lt;&gt;"",Compartments!$A276,"")</f>
         <v/>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" s="3" t="str">
         <f>IF(Compartments!$A277&lt;&gt;"",Compartments!$A277,"")</f>
         <v/>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" s="3" t="str">
         <f>IF(Compartments!$A278&lt;&gt;"",Compartments!$A278,"")</f>
         <v/>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" s="3" t="str">
         <f>IF(Compartments!$A279&lt;&gt;"",Compartments!$A279,"")</f>
         <v/>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" s="3" t="str">
         <f>IF(Compartments!$A280&lt;&gt;"",Compartments!$A280,"")</f>
         <v/>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" s="3" t="str">
         <f>IF(Compartments!$A281&lt;&gt;"",Compartments!$A281,"")</f>
         <v/>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" s="3" t="str">
         <f>IF(Compartments!$A282&lt;&gt;"",Compartments!$A282,"")</f>
         <v/>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" s="3" t="str">
         <f>IF(Compartments!$A283&lt;&gt;"",Compartments!$A283,"")</f>
         <v/>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" s="3" t="str">
         <f>IF(Compartments!$A284&lt;&gt;"",Compartments!$A284,"")</f>
         <v/>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285" s="3" t="str">
         <f>IF(Compartments!$A285&lt;&gt;"",Compartments!$A285,"")</f>
         <v/>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="3" t="str">
         <f>IF(Compartments!$A286&lt;&gt;"",Compartments!$A286,"")</f>
         <v/>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" s="3" t="str">
         <f>IF(Compartments!$A287&lt;&gt;"",Compartments!$A287,"")</f>
         <v/>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288" s="3" t="str">
         <f>IF(Compartments!$A288&lt;&gt;"",Compartments!$A288,"")</f>
         <v/>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" s="3" t="str">
         <f>IF(Compartments!$A289&lt;&gt;"",Compartments!$A289,"")</f>
         <v/>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" s="3" t="str">
         <f>IF(Compartments!$A290&lt;&gt;"",Compartments!$A290,"")</f>
         <v/>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A291" s="3" t="str">
         <f>IF(Compartments!$A291&lt;&gt;"",Compartments!$A291,"")</f>
         <v/>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" s="3" t="str">
         <f>IF(Compartments!$A292&lt;&gt;"",Compartments!$A292,"")</f>
         <v/>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293" s="3" t="str">
         <f>IF(Compartments!$A293&lt;&gt;"",Compartments!$A293,"")</f>
         <v/>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A294" s="3" t="str">
         <f>IF(Compartments!$A294&lt;&gt;"",Compartments!$A294,"")</f>
         <v/>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" s="3" t="str">
         <f>IF(Compartments!$A295&lt;&gt;"",Compartments!$A295,"")</f>
         <v/>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" s="3" t="str">
         <f>IF(Compartments!$A296&lt;&gt;"",Compartments!$A296,"")</f>
         <v/>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A297" s="3" t="str">
         <f>IF(Compartments!$A297&lt;&gt;"",Compartments!$A297,"")</f>
         <v/>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" s="3" t="str">
         <f>IF(Compartments!$A298&lt;&gt;"",Compartments!$A298,"")</f>
         <v/>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299" s="3" t="str">
         <f>IF(Compartments!$A299&lt;&gt;"",Compartments!$A299,"")</f>
         <v/>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" s="3" t="str">
         <f>IF(Compartments!$A300&lt;&gt;"",Compartments!$A300,"")</f>
         <v/>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" s="3" t="str">
         <f>IF(Compartments!$A301&lt;&gt;"",Compartments!$A301,"")</f>
         <v/>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302" s="3" t="str">
         <f>IF(Compartments!$A302&lt;&gt;"",Compartments!$A302,"")</f>
         <v/>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303" s="3" t="str">
         <f>IF(Compartments!$A303&lt;&gt;"",Compartments!$A303,"")</f>
         <v/>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" s="3" t="str">
         <f>IF(Compartments!$A304&lt;&gt;"",Compartments!$A304,"")</f>
         <v/>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305" s="3" t="str">
         <f>IF(Compartments!$A305&lt;&gt;"",Compartments!$A305,"")</f>
         <v/>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A306" s="3" t="str">
         <f>IF(Compartments!$A306&lt;&gt;"",Compartments!$A306,"")</f>
         <v/>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307" s="3" t="str">
         <f>IF(Compartments!$A307&lt;&gt;"",Compartments!$A307,"")</f>
         <v/>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" s="3" t="str">
         <f>IF(Compartments!$A308&lt;&gt;"",Compartments!$A308,"")</f>
         <v/>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A309" s="3" t="str">
         <f>IF(Compartments!$A309&lt;&gt;"",Compartments!$A309,"")</f>
         <v/>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A310" s="3" t="str">
         <f>IF(Compartments!$A310&lt;&gt;"",Compartments!$A310,"")</f>
         <v/>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A311" s="3" t="str">
         <f>IF(Compartments!$A311&lt;&gt;"",Compartments!$A311,"")</f>
         <v/>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A312" s="3" t="str">
         <f>IF(Compartments!$A312&lt;&gt;"",Compartments!$A312,"")</f>
         <v/>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A313" s="3" t="str">
         <f>IF(Compartments!$A313&lt;&gt;"",Compartments!$A313,"")</f>
         <v/>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314" s="3" t="str">
         <f>IF(Compartments!$A314&lt;&gt;"",Compartments!$A314,"")</f>
         <v/>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A315" s="3" t="str">
         <f>IF(Compartments!$A315&lt;&gt;"",Compartments!$A315,"")</f>
         <v/>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" s="3" t="str">
         <f>IF(Compartments!$A316&lt;&gt;"",Compartments!$A316,"")</f>
         <v/>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317" s="3" t="str">
         <f>IF(Compartments!$A317&lt;&gt;"",Compartments!$A317,"")</f>
         <v/>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" s="3" t="str">
         <f>IF(Compartments!$A318&lt;&gt;"",Compartments!$A318,"")</f>
         <v/>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A319" s="3" t="str">
         <f>IF(Compartments!$A319&lt;&gt;"",Compartments!$A319,"")</f>
         <v/>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A320" s="3" t="str">
         <f>IF(Compartments!$A320&lt;&gt;"",Compartments!$A320,"")</f>
         <v/>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A321" s="3" t="str">
         <f>IF(Compartments!$A321&lt;&gt;"",Compartments!$A321,"")</f>
         <v/>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" s="3" t="str">
         <f>IF(Compartments!$A322&lt;&gt;"",Compartments!$A322,"")</f>
         <v/>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323" s="3" t="str">
         <f>IF(Compartments!$A323&lt;&gt;"",Compartments!$A323,"")</f>
         <v/>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A324" s="3" t="str">
         <f>IF(Compartments!$A324&lt;&gt;"",Compartments!$A324,"")</f>
         <v/>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" s="3" t="str">
         <f>IF(Compartments!$A325&lt;&gt;"",Compartments!$A325,"")</f>
         <v/>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A326" s="3" t="str">
         <f>IF(Compartments!$A326&lt;&gt;"",Compartments!$A326,"")</f>
         <v/>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A327" s="3" t="str">
         <f>IF(Compartments!$A327&lt;&gt;"",Compartments!$A327,"")</f>
         <v/>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A328" s="3" t="str">
         <f>IF(Compartments!$A328&lt;&gt;"",Compartments!$A328,"")</f>
         <v/>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A329" s="3" t="str">
         <f>IF(Compartments!$A329&lt;&gt;"",Compartments!$A329,"")</f>
         <v/>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A330" s="3" t="str">
         <f>IF(Compartments!$A330&lt;&gt;"",Compartments!$A330,"")</f>
         <v/>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" s="3" t="str">
         <f>IF(Compartments!$A331&lt;&gt;"",Compartments!$A331,"")</f>
         <v/>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" s="3" t="str">
         <f>IF(Compartments!$A332&lt;&gt;"",Compartments!$A332,"")</f>
         <v/>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" s="3" t="str">
         <f>IF(Compartments!$A333&lt;&gt;"",Compartments!$A333,"")</f>
         <v/>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A334" s="3" t="str">
         <f>IF(Compartments!$A334&lt;&gt;"",Compartments!$A334,"")</f>
         <v/>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A335" s="3" t="str">
         <f>IF(Compartments!$A335&lt;&gt;"",Compartments!$A335,"")</f>
         <v/>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A336" s="3" t="str">
         <f>IF(Compartments!$A336&lt;&gt;"",Compartments!$A336,"")</f>
         <v/>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" s="3" t="str">
         <f>IF(Compartments!$A337&lt;&gt;"",Compartments!$A337,"")</f>
         <v/>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" s="3" t="str">
         <f>IF(Compartments!$A338&lt;&gt;"",Compartments!$A338,"")</f>
         <v/>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" s="3" t="str">
         <f>IF(Compartments!$A339&lt;&gt;"",Compartments!$A339,"")</f>
         <v/>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" s="3" t="str">
         <f>IF(Compartments!$A340&lt;&gt;"",Compartments!$A340,"")</f>
         <v/>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341" s="3" t="str">
         <f>IF(Compartments!$A341&lt;&gt;"",Compartments!$A341,"")</f>
         <v/>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A342" s="3" t="str">
         <f>IF(Compartments!$A342&lt;&gt;"",Compartments!$A342,"")</f>
         <v/>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343" s="3" t="str">
         <f>IF(Compartments!$A343&lt;&gt;"",Compartments!$A343,"")</f>
         <v/>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" s="3" t="str">
         <f>IF(Compartments!$A344&lt;&gt;"",Compartments!$A344,"")</f>
         <v/>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A345" s="3" t="str">
         <f>IF(Compartments!$A345&lt;&gt;"",Compartments!$A345,"")</f>
         <v/>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" s="3" t="str">
         <f>IF(Compartments!$A346&lt;&gt;"",Compartments!$A346,"")</f>
         <v/>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347" s="3" t="str">
         <f>IF(Compartments!$A347&lt;&gt;"",Compartments!$A347,"")</f>
         <v/>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A348" s="3" t="str">
         <f>IF(Compartments!$A348&lt;&gt;"",Compartments!$A348,"")</f>
         <v/>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" s="3" t="str">
         <f>IF(Compartments!$A349&lt;&gt;"",Compartments!$A349,"")</f>
         <v/>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" s="3" t="str">
         <f>IF(Compartments!$A350&lt;&gt;"",Compartments!$A350,"")</f>
         <v/>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A351" s="3" t="str">
         <f>IF(Compartments!$A351&lt;&gt;"",Compartments!$A351,"")</f>
         <v/>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A352" s="3" t="str">
         <f>IF(Compartments!$A352&lt;&gt;"",Compartments!$A352,"")</f>
         <v/>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" s="3" t="str">
         <f>IF(Compartments!$A353&lt;&gt;"",Compartments!$A353,"")</f>
         <v/>
       </c>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A354" s="3" t="str">
         <f>IF(Compartments!$A354&lt;&gt;"",Compartments!$A354,"")</f>
         <v/>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" s="3" t="str">
         <f>IF(Compartments!$A355&lt;&gt;"",Compartments!$A355,"")</f>
         <v/>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A356" s="3" t="str">
         <f>IF(Compartments!$A356&lt;&gt;"",Compartments!$A356,"")</f>
         <v/>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A357" s="3" t="str">
         <f>IF(Compartments!$A357&lt;&gt;"",Compartments!$A357,"")</f>
         <v/>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" s="3" t="str">
         <f>IF(Compartments!$A358&lt;&gt;"",Compartments!$A358,"")</f>
         <v/>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" s="3" t="str">
         <f>IF(Compartments!$A359&lt;&gt;"",Compartments!$A359,"")</f>
         <v/>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" s="3" t="str">
         <f>IF(Compartments!$A360&lt;&gt;"",Compartments!$A360,"")</f>
         <v/>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A361" s="3" t="str">
         <f>IF(Compartments!$A361&lt;&gt;"",Compartments!$A361,"")</f>
         <v/>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" s="3" t="str">
         <f>IF(Compartments!$A362&lt;&gt;"",Compartments!$A362,"")</f>
         <v/>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" s="3" t="str">
         <f>IF(Compartments!$A363&lt;&gt;"",Compartments!$A363,"")</f>
         <v/>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" s="3" t="str">
         <f>IF(Compartments!$A364&lt;&gt;"",Compartments!$A364,"")</f>
         <v/>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" s="3" t="str">
         <f>IF(Compartments!$A365&lt;&gt;"",Compartments!$A365,"")</f>
         <v/>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A366" s="3" t="str">
         <f>IF(Compartments!$A366&lt;&gt;"",Compartments!$A366,"")</f>
         <v/>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A367" s="3" t="str">
         <f>IF(Compartments!$A367&lt;&gt;"",Compartments!$A367,"")</f>
         <v/>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" s="3" t="str">
         <f>IF(Compartments!$A368&lt;&gt;"",Compartments!$A368,"")</f>
         <v/>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A369" s="3" t="str">
         <f>IF(Compartments!$A369&lt;&gt;"",Compartments!$A369,"")</f>
         <v/>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370" s="3" t="str">
         <f>IF(Compartments!$A370&lt;&gt;"",Compartments!$A370,"")</f>
         <v/>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" s="3" t="str">
         <f>IF(Compartments!$A371&lt;&gt;"",Compartments!$A371,"")</f>
         <v/>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A372" s="3" t="str">
         <f>IF(Compartments!$A372&lt;&gt;"",Compartments!$A372,"")</f>
         <v/>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A373" s="3" t="str">
         <f>IF(Compartments!$A373&lt;&gt;"",Compartments!$A373,"")</f>
         <v/>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" s="3" t="str">
         <f>IF(Compartments!$A374&lt;&gt;"",Compartments!$A374,"")</f>
         <v/>
       </c>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" s="3" t="str">
         <f>IF(Compartments!$A375&lt;&gt;"",Compartments!$A375,"")</f>
         <v/>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" s="3" t="str">
         <f>IF(Compartments!$A376&lt;&gt;"",Compartments!$A376,"")</f>
         <v/>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" s="3" t="str">
         <f>IF(Compartments!$A377&lt;&gt;"",Compartments!$A377,"")</f>
         <v/>
       </c>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" s="3" t="str">
         <f>IF(Compartments!$A378&lt;&gt;"",Compartments!$A378,"")</f>
         <v/>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" s="3" t="str">
         <f>IF(Compartments!$A379&lt;&gt;"",Compartments!$A379,"")</f>
         <v/>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" s="3" t="str">
         <f>IF(Compartments!$A380&lt;&gt;"",Compartments!$A380,"")</f>
         <v/>
       </c>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381" s="3" t="str">
         <f>IF(Compartments!$A381&lt;&gt;"",Compartments!$A381,"")</f>
         <v/>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" s="3" t="str">
         <f>IF(Compartments!$A382&lt;&gt;"",Compartments!$A382,"")</f>
         <v/>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" s="3" t="str">
         <f>IF(Compartments!$A383&lt;&gt;"",Compartments!$A383,"")</f>
         <v/>
       </c>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A384" s="3" t="str">
         <f>IF(Compartments!$A384&lt;&gt;"",Compartments!$A384,"")</f>
         <v/>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" s="3" t="str">
         <f>IF(Compartments!$A385&lt;&gt;"",Compartments!$A385,"")</f>
         <v/>
       </c>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A386" s="3" t="str">
         <f>IF(Compartments!$A386&lt;&gt;"",Compartments!$A386,"")</f>
         <v/>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A387" s="3" t="str">
         <f>IF(Compartments!$A387&lt;&gt;"",Compartments!$A387,"")</f>
         <v/>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A388" s="3" t="str">
         <f>IF(Compartments!$A388&lt;&gt;"",Compartments!$A388,"")</f>
         <v/>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A389" s="3" t="str">
         <f>IF(Compartments!$A389&lt;&gt;"",Compartments!$A389,"")</f>
         <v/>
       </c>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A390" s="3" t="str">
         <f>IF(Compartments!$A390&lt;&gt;"",Compartments!$A390,"")</f>
         <v/>
       </c>
     </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A391" s="3" t="str">
         <f>IF(Compartments!$A391&lt;&gt;"",Compartments!$A391,"")</f>
         <v/>
       </c>
     </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A392" s="3" t="str">
         <f>IF(Compartments!$A392&lt;&gt;"",Compartments!$A392,"")</f>
         <v/>
       </c>
     </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A393" s="3" t="str">
         <f>IF(Compartments!$A393&lt;&gt;"",Compartments!$A393,"")</f>
         <v/>
       </c>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A394" s="3" t="str">
         <f>IF(Compartments!$A394&lt;&gt;"",Compartments!$A394,"")</f>
         <v/>
       </c>
     </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" s="3" t="str">
         <f>IF(Compartments!$A395&lt;&gt;"",Compartments!$A395,"")</f>
         <v/>
       </c>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" s="3" t="str">
         <f>IF(Compartments!$A396&lt;&gt;"",Compartments!$A396,"")</f>
         <v/>
       </c>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" s="3" t="str">
         <f>IF(Compartments!$A397&lt;&gt;"",Compartments!$A397,"")</f>
         <v/>
       </c>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" s="3" t="str">
         <f>IF(Compartments!$A398&lt;&gt;"",Compartments!$A398,"")</f>
         <v/>
@@ -6040,16 +6077,16 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="6" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="6" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6066,7 +6103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -6115,7 +6152,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B08FC4CC-1E7B-E34A-9FEC-BBB85EF18DBD}">
           <x14:formula1>
-            <xm:f>'[framework_template_advanced.xlsx]Databook Pages'!#REF!</xm:f>
+            <xm:f>'E:\projects\atomica\atomica\atomica\[framework_template_advanced.xlsx]Databook Pages'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E1</xm:sqref>
         </x14:dataValidation>
@@ -6136,18 +6173,18 @@
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" customWidth="1"/>
-    <col min="4" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
+    <col min="4" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6176,7 +6213,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -6195,7 +6232,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6240,7 +6277,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1EB69DA7-5FD8-0D4F-B979-35948680D928}">
           <x14:formula1>
-            <xm:f>'[framework_template_advanced.xlsx]Databook Pages'!#REF!</xm:f>
+            <xm:f>'E:\projects\atomica\atomica\atomica\[framework_template_advanced.xlsx]Databook Pages'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>I1</xm:sqref>
         </x14:dataValidation>
@@ -6254,16 +6291,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45475D22-3C2C-420F-8B01-74A730C6AAB5}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.83203125" customWidth="1"/>
+    <col min="1" max="2" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>24</v>
       </c>
@@ -6271,10 +6308,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
     </row>
   </sheetData>

</xml_diff>